<commit_message>
Added myc translocation info
</commit_message>
<xml_diff>
--- a/1_Input/Sample_overview.xlsx
+++ b/1_Input/Sample_overview.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.s.steemers/surfdrive/Shared/pmc_vanboxtel/projects/Lymphoma_scWGS/1_Input/Burkitt_paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.s.steemers/surfdrive/Shared/pmc_vanboxtel/projects/Burkitt_github/1_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92CA9E4-DE48-EE49-B071-4E2BFDE52D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C399DE3-8376-734D-B372-1A854C73FA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22660" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{42CF7DF2-1AE8-0C4E-8116-5678FAC88E91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6271" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6375" uniqueCount="426">
   <si>
     <t>Sample_name</t>
   </si>
@@ -1311,6 +1311,12 @@
   </si>
   <si>
     <t>N/a</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1430,6 +1436,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1767,15 +1782,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA242BA5-733B-FC49-A2B2-17B2B6C5E9F6}">
-  <dimension ref="A1:AR346"/>
+  <dimension ref="A1:AR361"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -2005,6 +2023,9 @@
       <c r="Q2" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R2" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S2" s="14">
         <v>0.96916100000000005</v>
       </c>
@@ -2014,10 +2035,10 @@
       <c r="U2" s="14">
         <v>18.541861999999998</v>
       </c>
-      <c r="V2" s="13">
+      <c r="V2" s="17">
         <v>2382265274</v>
       </c>
-      <c r="W2" s="1">
+      <c r="W2" s="16">
         <f>V2/2745186691</f>
         <v>0.86779718181287069</v>
       </c>
@@ -2102,6 +2123,9 @@
       <c r="Q3" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R3" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S3" s="14">
         <v>0.96761900000000001</v>
       </c>
@@ -2111,10 +2135,10 @@
       <c r="U3" s="14">
         <v>21.387689999999999</v>
       </c>
-      <c r="V3" s="13">
+      <c r="V3" s="17">
         <v>2429729351</v>
       </c>
-      <c r="W3" s="1">
+      <c r="W3" s="16">
         <f t="shared" ref="W3:W66" si="0">V3/2745186691</f>
         <v>0.88508710863482765</v>
       </c>
@@ -2199,6 +2223,9 @@
       <c r="Q4" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R4" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S4" s="14">
         <v>0.96490299999999996</v>
       </c>
@@ -2208,10 +2235,10 @@
       <c r="U4" s="14">
         <v>14.929095999999999</v>
       </c>
-      <c r="V4" s="13">
+      <c r="V4" s="17">
         <v>2273742795</v>
       </c>
-      <c r="W4" s="1">
+      <c r="W4" s="16">
         <f t="shared" si="0"/>
         <v>0.8282652697007411</v>
       </c>
@@ -2296,6 +2323,9 @@
       <c r="Q5" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R5" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S5" s="14">
         <v>0.96772800000000003</v>
       </c>
@@ -2305,10 +2335,10 @@
       <c r="U5" s="14">
         <v>20.630858</v>
       </c>
-      <c r="V5" s="13">
+      <c r="V5" s="17">
         <v>2471367600</v>
       </c>
-      <c r="W5" s="1">
+      <c r="W5" s="16">
         <f t="shared" si="0"/>
         <v>0.9002548380779688</v>
       </c>
@@ -2393,6 +2423,9 @@
       <c r="Q6" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R6" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S6" s="14">
         <v>0.96809299999999998</v>
       </c>
@@ -2402,10 +2435,10 @@
       <c r="U6" s="14">
         <v>19.542511000000001</v>
       </c>
-      <c r="V6" s="13">
+      <c r="V6" s="17">
         <v>2460969547</v>
       </c>
-      <c r="W6" s="1">
+      <c r="W6" s="16">
         <f t="shared" si="0"/>
         <v>0.89646709823714499</v>
       </c>
@@ -2490,6 +2523,9 @@
       <c r="Q7" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R7" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S7" s="14">
         <v>0.96806000000000003</v>
       </c>
@@ -2499,10 +2535,10 @@
       <c r="U7" s="14">
         <v>18.084444999999999</v>
       </c>
-      <c r="V7" s="13">
+      <c r="V7" s="17">
         <v>2344170295</v>
       </c>
-      <c r="W7" s="1">
+      <c r="W7" s="16">
         <f t="shared" si="0"/>
         <v>0.85392017332929726</v>
       </c>
@@ -2587,6 +2623,9 @@
       <c r="Q8" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R8" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S8" s="14">
         <v>0.96821400000000002</v>
       </c>
@@ -2596,10 +2635,10 @@
       <c r="U8" s="14">
         <v>15.716710000000001</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="17">
         <v>2358976325</v>
       </c>
-      <c r="W8" s="1">
+      <c r="W8" s="16">
         <f t="shared" si="0"/>
         <v>0.85931362436435477</v>
       </c>
@@ -2684,6 +2723,9 @@
       <c r="Q9" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R9" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S9" s="14">
         <v>0.96718999999999999</v>
       </c>
@@ -2693,10 +2735,10 @@
       <c r="U9" s="14">
         <v>15.111796</v>
       </c>
-      <c r="V9" s="13">
+      <c r="V9" s="17">
         <v>2226569422</v>
       </c>
-      <c r="W9" s="1">
+      <c r="W9" s="16">
         <f t="shared" si="0"/>
         <v>0.81108123877320659</v>
       </c>
@@ -2781,6 +2823,9 @@
       <c r="Q10" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R10" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S10" s="14">
         <v>0.96650100000000005</v>
       </c>
@@ -2790,10 +2835,10 @@
       <c r="U10" s="14">
         <v>13.151318</v>
       </c>
-      <c r="V10" s="13">
+      <c r="V10" s="17">
         <v>2256669463</v>
       </c>
-      <c r="W10" s="1">
+      <c r="W10" s="16">
         <f t="shared" si="0"/>
         <v>0.82204589960982</v>
       </c>
@@ -2878,6 +2923,9 @@
       <c r="Q11" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R11" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S11" s="14">
         <v>0.96816599999999997</v>
       </c>
@@ -2887,10 +2935,10 @@
       <c r="U11" s="14">
         <v>13.878892</v>
       </c>
-      <c r="V11" s="13">
+      <c r="V11" s="17">
         <v>2264135273</v>
       </c>
-      <c r="W11" s="1">
+      <c r="W11" s="16">
         <f t="shared" si="0"/>
         <v>0.82476549971005231</v>
       </c>
@@ -2975,6 +3023,9 @@
       <c r="Q12" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R12" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S12" s="14">
         <v>0.96503799999999995</v>
       </c>
@@ -2984,10 +3035,10 @@
       <c r="U12" s="14">
         <v>12.794624000000001</v>
       </c>
-      <c r="V12" s="13">
+      <c r="V12" s="17">
         <v>2110761189</v>
       </c>
-      <c r="W12" s="1">
+      <c r="W12" s="16">
         <f t="shared" si="0"/>
         <v>0.76889531627122409</v>
       </c>
@@ -3072,6 +3123,9 @@
       <c r="Q13" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R13" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S13" s="14">
         <v>0.94896100000000005</v>
       </c>
@@ -3081,10 +3135,10 @@
       <c r="U13" s="14">
         <v>13.600479999999999</v>
       </c>
-      <c r="V13" s="13">
+      <c r="V13" s="17">
         <v>2032531729</v>
       </c>
-      <c r="W13" s="1">
+      <c r="W13" s="16">
         <f t="shared" si="0"/>
         <v>0.74039836185407182</v>
       </c>
@@ -3169,6 +3223,9 @@
       <c r="Q14" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R14" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S14" s="14">
         <v>0.96870000000000001</v>
       </c>
@@ -3178,10 +3235,10 @@
       <c r="U14" s="14">
         <v>15.48151</v>
       </c>
-      <c r="V14" s="13">
+      <c r="V14" s="17">
         <v>2365930766</v>
       </c>
-      <c r="W14" s="1">
+      <c r="W14" s="16">
         <f t="shared" si="0"/>
         <v>0.86184694605894108</v>
       </c>
@@ -3266,6 +3323,9 @@
       <c r="Q15" s="1" t="s">
         <v>422</v>
       </c>
+      <c r="R15" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S15" s="14">
         <v>0.93301800000000001</v>
       </c>
@@ -3275,10 +3335,10 @@
       <c r="U15" s="14">
         <v>11.860697999999999</v>
       </c>
-      <c r="V15" s="13">
+      <c r="V15" s="17">
         <v>1786040209</v>
       </c>
-      <c r="W15" s="1">
+      <c r="W15" s="16">
         <f t="shared" si="0"/>
         <v>0.6506079221699097</v>
       </c>
@@ -3363,6 +3423,9 @@
       <c r="Q16" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R16" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S16" s="14">
         <v>0.95537099999999997</v>
       </c>
@@ -3372,10 +3435,10 @@
       <c r="U16" s="14">
         <v>11.520887</v>
       </c>
-      <c r="V16" s="13">
+      <c r="V16" s="17">
         <v>1759474788</v>
       </c>
-      <c r="W16" s="1">
+      <c r="W16" s="16">
         <f t="shared" si="0"/>
         <v>0.64093083132319473</v>
       </c>
@@ -3460,6 +3523,9 @@
       <c r="Q17" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R17" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S17" s="14">
         <v>0.96361200000000002</v>
       </c>
@@ -3469,10 +3535,10 @@
       <c r="U17" s="14">
         <v>14.298394999999999</v>
       </c>
-      <c r="V17" s="13">
+      <c r="V17" s="17">
         <v>2134959893</v>
       </c>
-      <c r="W17" s="1">
+      <c r="W17" s="16">
         <f t="shared" si="0"/>
         <v>0.77771027376731516</v>
       </c>
@@ -3557,6 +3623,9 @@
       <c r="Q18" s="1" t="s">
         <v>422</v>
       </c>
+      <c r="R18" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S18" s="14">
         <v>0.75931599999999999</v>
       </c>
@@ -3566,10 +3635,10 @@
       <c r="U18" s="14">
         <v>14.294221</v>
       </c>
-      <c r="V18" s="13">
+      <c r="V18" s="17">
         <v>1639386564</v>
       </c>
-      <c r="W18" s="1">
+      <c r="W18" s="16">
         <f t="shared" si="0"/>
         <v>0.59718581959277028</v>
       </c>
@@ -3653,6 +3722,9 @@
       <c r="Q19" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R19" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S19" s="14">
         <v>0.96423499999999995</v>
       </c>
@@ -3662,10 +3734,10 @@
       <c r="U19" s="14">
         <v>16.085729000000001</v>
       </c>
-      <c r="V19" s="13">
+      <c r="V19" s="17">
         <v>2336009052</v>
       </c>
-      <c r="W19" s="1">
+      <c r="W19" s="16">
         <f t="shared" si="0"/>
         <v>0.8509472451030472</v>
       </c>
@@ -3750,6 +3822,9 @@
       <c r="Q20" s="1" t="s">
         <v>422</v>
       </c>
+      <c r="R20" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S20" s="14">
         <v>0.55152900000000005</v>
       </c>
@@ -3759,10 +3834,10 @@
       <c r="U20" s="14">
         <v>11.758459999999999</v>
       </c>
-      <c r="V20" s="13">
+      <c r="V20" s="17">
         <v>819503888</v>
       </c>
-      <c r="W20" s="1">
+      <c r="W20" s="16">
         <f t="shared" si="0"/>
         <v>0.29852391849585869</v>
       </c>
@@ -3846,6 +3921,9 @@
       <c r="Q21" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R21" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S21" s="14">
         <v>0.944052</v>
       </c>
@@ -3855,10 +3933,10 @@
       <c r="U21" s="14">
         <v>19.989332000000001</v>
       </c>
-      <c r="V21" s="13">
+      <c r="V21" s="17">
         <v>2115959536</v>
       </c>
-      <c r="W21" s="1">
+      <c r="W21" s="16">
         <f t="shared" si="0"/>
         <v>0.77078893866748677</v>
       </c>
@@ -3943,6 +4021,9 @@
       <c r="Q22" s="1" t="s">
         <v>422</v>
       </c>
+      <c r="R22" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S22" s="14">
         <v>0.52857900000000002</v>
       </c>
@@ -3952,10 +4033,10 @@
       <c r="U22" s="14">
         <v>11.342373</v>
       </c>
-      <c r="V22" s="13">
+      <c r="V22" s="17">
         <v>790473543</v>
       </c>
-      <c r="W22" s="1">
+      <c r="W22" s="16">
         <f t="shared" si="0"/>
         <v>0.28794892004669126</v>
       </c>
@@ -4039,6 +4120,9 @@
       <c r="Q23" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="R23" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S23" s="14">
         <v>0.97236100000000003</v>
       </c>
@@ -4048,10 +4132,10 @@
       <c r="U23" s="14">
         <v>27.547062</v>
       </c>
-      <c r="V23" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="W23" s="1" t="e">
+      <c r="V23" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="W23" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -4135,6 +4219,9 @@
       <c r="Q24" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R24" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S24" s="13">
         <v>0.96920799999999996</v>
       </c>
@@ -4144,10 +4231,10 @@
       <c r="U24" s="13">
         <v>22.680377</v>
       </c>
-      <c r="V24" s="13">
+      <c r="V24" s="17">
         <v>2613347583</v>
       </c>
-      <c r="W24" s="1">
+      <c r="W24" s="16">
         <f t="shared" si="0"/>
         <v>0.95197444733641245</v>
       </c>
@@ -4231,6 +4318,9 @@
       <c r="Q25" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R25" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S25" s="13">
         <v>0.93278300000000003</v>
       </c>
@@ -4240,10 +4330,10 @@
       <c r="U25" s="13">
         <v>10.124105</v>
       </c>
-      <c r="V25" s="13">
+      <c r="V25" s="17">
         <v>1708556401</v>
       </c>
-      <c r="W25" s="1">
+      <c r="W25" s="16">
         <f t="shared" si="0"/>
         <v>0.62238258935228097</v>
       </c>
@@ -4327,6 +4417,9 @@
       <c r="Q26" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R26" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S26" s="13">
         <v>0.90099399999999996</v>
       </c>
@@ -4336,10 +4429,10 @@
       <c r="U26" s="13">
         <v>11.45749</v>
       </c>
-      <c r="V26" s="13">
+      <c r="V26" s="17">
         <v>1744627241</v>
       </c>
-      <c r="W26" s="1">
+      <c r="W26" s="16">
         <f t="shared" si="0"/>
         <v>0.63552225672654628</v>
       </c>
@@ -4423,6 +4516,9 @@
       <c r="Q27" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R27" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S27" s="13">
         <v>0.95354700000000003</v>
       </c>
@@ -4432,10 +4528,10 @@
       <c r="U27" s="13">
         <v>11.342556</v>
       </c>
-      <c r="V27" s="13">
+      <c r="V27" s="17">
         <v>1904813773</v>
       </c>
-      <c r="W27" s="1">
+      <c r="W27" s="16">
         <f t="shared" si="0"/>
         <v>0.69387403750894838</v>
       </c>
@@ -4519,6 +4615,9 @@
       <c r="Q28" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R28" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S28" s="13">
         <v>0.95572400000000002</v>
       </c>
@@ -4528,10 +4627,10 @@
       <c r="U28" s="13">
         <v>10.532508999999999</v>
       </c>
-      <c r="V28" s="13">
+      <c r="V28" s="17">
         <v>1767620755</v>
       </c>
-      <c r="W28" s="1">
+      <c r="W28" s="16">
         <f t="shared" si="0"/>
         <v>0.64389819490058131</v>
       </c>
@@ -4615,6 +4714,9 @@
       <c r="Q29" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R29" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S29" s="13">
         <v>0.95258200000000004</v>
       </c>
@@ -4624,10 +4726,10 @@
       <c r="U29" s="13">
         <v>9.6453579999999999</v>
       </c>
-      <c r="V29" s="13">
+      <c r="V29" s="17">
         <v>1648441203</v>
       </c>
-      <c r="W29" s="1">
+      <c r="W29" s="16">
         <f t="shared" si="0"/>
         <v>0.60048418870904396</v>
       </c>
@@ -4711,6 +4813,9 @@
       <c r="Q30" s="1" t="s">
         <v>422</v>
       </c>
+      <c r="R30" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S30" s="13">
         <v>0.93830499999999994</v>
       </c>
@@ -4720,10 +4825,10 @@
       <c r="U30" s="13">
         <v>9.0467829999999996</v>
       </c>
-      <c r="V30" s="13">
+      <c r="V30" s="17">
         <v>1524316944</v>
       </c>
-      <c r="W30" s="1">
+      <c r="W30" s="16">
         <f t="shared" si="0"/>
         <v>0.55526895456597569</v>
       </c>
@@ -4807,6 +4912,9 @@
       <c r="Q31" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R31" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S31" s="13">
         <v>0.95080200000000004</v>
       </c>
@@ -4816,10 +4924,10 @@
       <c r="U31" s="13">
         <v>15.529591</v>
       </c>
-      <c r="V31" s="13">
+      <c r="V31" s="17">
         <v>2150350435</v>
       </c>
-      <c r="W31" s="1">
+      <c r="W31" s="16">
         <f>V31/2745186691</f>
         <v>0.78331664729755901</v>
       </c>
@@ -4903,6 +5011,9 @@
       <c r="Q32" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R32" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S32" s="13">
         <v>0.90756499999999996</v>
       </c>
@@ -4912,10 +5023,10 @@
       <c r="U32" s="13">
         <v>11.603737000000001</v>
       </c>
-      <c r="V32" s="13">
+      <c r="V32" s="17">
         <v>1821804526</v>
       </c>
-      <c r="W32" s="1">
+      <c r="W32" s="16">
         <f t="shared" si="0"/>
         <v>0.6636359312001342</v>
       </c>
@@ -4999,6 +5110,9 @@
       <c r="Q33" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R33" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S33" s="13">
         <v>0.96198399999999995</v>
       </c>
@@ -5008,10 +5122,10 @@
       <c r="U33" s="13">
         <v>11.52768</v>
       </c>
-      <c r="V33" s="13">
+      <c r="V33" s="17">
         <v>2069570328</v>
       </c>
-      <c r="W33" s="1">
+      <c r="W33" s="16">
         <f t="shared" si="0"/>
         <v>0.75389055862212029</v>
       </c>
@@ -5095,6 +5209,9 @@
       <c r="Q34" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R34" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S34" s="13">
         <v>0.95821699999999999</v>
       </c>
@@ -5104,10 +5221,10 @@
       <c r="U34" s="13">
         <v>10.729044999999999</v>
       </c>
-      <c r="V34" s="13">
+      <c r="V34" s="17">
         <v>1901447996</v>
       </c>
-      <c r="W34" s="1">
+      <c r="W34" s="16">
         <f t="shared" si="0"/>
         <v>0.69264797262562572</v>
       </c>
@@ -5191,6 +5308,9 @@
       <c r="Q35" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R35" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S35" s="13">
         <v>0.95325899999999997</v>
       </c>
@@ -5200,10 +5320,10 @@
       <c r="U35" s="13">
         <v>12.037646000000001</v>
       </c>
-      <c r="V35" s="13">
+      <c r="V35" s="17">
         <v>1805967881</v>
       </c>
-      <c r="W35" s="1">
+      <c r="W35" s="16">
         <f t="shared" si="0"/>
         <v>0.65786705396787892</v>
       </c>
@@ -5287,6 +5407,9 @@
       <c r="Q36" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R36" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S36" s="13">
         <v>0.94850699999999999</v>
       </c>
@@ -5296,10 +5419,10 @@
       <c r="U36" s="13">
         <v>8.739808</v>
       </c>
-      <c r="V36" s="13">
+      <c r="V36" s="17">
         <v>1507302843</v>
       </c>
-      <c r="W36" s="1">
+      <c r="W36" s="16">
         <f t="shared" si="0"/>
         <v>0.54907116078539953</v>
       </c>
@@ -5383,6 +5506,9 @@
       <c r="Q37" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R37" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S37" s="13">
         <v>0.95750500000000005</v>
       </c>
@@ -5392,10 +5518,10 @@
       <c r="U37" s="13">
         <v>11.050922</v>
       </c>
-      <c r="V37" s="13">
+      <c r="V37" s="17">
         <v>1878934461</v>
       </c>
-      <c r="W37" s="1">
+      <c r="W37" s="16">
         <f t="shared" si="0"/>
         <v>0.68444687829793938</v>
       </c>
@@ -5479,6 +5605,9 @@
       <c r="Q38" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R38" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S38" s="13">
         <v>0.94247300000000001</v>
       </c>
@@ -5488,10 +5617,10 @@
       <c r="U38" s="13">
         <v>11.518345999999999</v>
       </c>
-      <c r="V38" s="13">
+      <c r="V38" s="17">
         <v>1753157026</v>
       </c>
-      <c r="W38" s="1">
+      <c r="W38" s="16">
         <f t="shared" si="0"/>
         <v>0.63862943520295534</v>
       </c>
@@ -5569,7 +5698,8 @@
       <c r="O39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W39" s="1">
+      <c r="V39" s="18"/>
+      <c r="W39" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5647,7 +5777,8 @@
       <c r="O40" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W40" s="1">
+      <c r="V40" s="18"/>
+      <c r="W40" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5725,7 +5856,8 @@
       <c r="O41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W41" s="1">
+      <c r="V41" s="18"/>
+      <c r="W41" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5803,7 +5935,8 @@
       <c r="O42" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W42" s="1">
+      <c r="V42" s="18"/>
+      <c r="W42" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5881,7 +6014,8 @@
       <c r="O43" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W43" s="1">
+      <c r="V43" s="18"/>
+      <c r="W43" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5959,7 +6093,8 @@
       <c r="O44" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W44" s="1">
+      <c r="V44" s="18"/>
+      <c r="W44" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6037,7 +6172,8 @@
       <c r="O45" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W45" s="1">
+      <c r="V45" s="18"/>
+      <c r="W45" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6115,7 +6251,8 @@
       <c r="O46" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W46" s="1">
+      <c r="V46" s="18"/>
+      <c r="W46" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6193,7 +6330,8 @@
       <c r="O47" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W47" s="1">
+      <c r="V47" s="18"/>
+      <c r="W47" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6271,7 +6409,8 @@
       <c r="O48" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W48" s="1">
+      <c r="V48" s="18"/>
+      <c r="W48" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6349,7 +6488,8 @@
       <c r="O49" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W49" s="1">
+      <c r="V49" s="18"/>
+      <c r="W49" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6427,7 +6567,8 @@
       <c r="O50" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W50" s="1">
+      <c r="V50" s="18"/>
+      <c r="W50" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6505,7 +6646,8 @@
       <c r="O51" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W51" s="1">
+      <c r="V51" s="18"/>
+      <c r="W51" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6583,7 +6725,8 @@
       <c r="O52" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W52" s="1">
+      <c r="V52" s="18"/>
+      <c r="W52" s="16">
         <f>V52/2745186691</f>
         <v>0</v>
       </c>
@@ -6661,7 +6804,8 @@
       <c r="O53" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W53" s="1">
+      <c r="V53" s="18"/>
+      <c r="W53" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6739,7 +6883,8 @@
       <c r="O54" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W54" s="1">
+      <c r="V54" s="18"/>
+      <c r="W54" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6817,7 +6962,8 @@
       <c r="O55" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W55" s="1">
+      <c r="V55" s="18"/>
+      <c r="W55" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6895,7 +7041,8 @@
       <c r="O56" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W56" s="1">
+      <c r="V56" s="18"/>
+      <c r="W56" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6973,7 +7120,8 @@
       <c r="O57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W57" s="1">
+      <c r="V57" s="18"/>
+      <c r="W57" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7051,7 +7199,8 @@
       <c r="O58" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W58" s="1">
+      <c r="V58" s="18"/>
+      <c r="W58" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7129,7 +7278,8 @@
       <c r="O59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W59" s="1">
+      <c r="V59" s="18"/>
+      <c r="W59" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7207,7 +7357,8 @@
       <c r="O60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W60" s="1">
+      <c r="V60" s="18"/>
+      <c r="W60" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7285,7 +7436,8 @@
       <c r="O61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W61" s="1">
+      <c r="V61" s="18"/>
+      <c r="W61" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7363,7 +7515,8 @@
       <c r="O62" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W62" s="1">
+      <c r="V62" s="18"/>
+      <c r="W62" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7441,7 +7594,8 @@
       <c r="O63" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W63" s="1">
+      <c r="V63" s="18"/>
+      <c r="W63" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7519,7 +7673,8 @@
       <c r="O64" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W64" s="1">
+      <c r="V64" s="18"/>
+      <c r="W64" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7597,7 +7752,8 @@
       <c r="O65" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W65" s="1">
+      <c r="V65" s="18"/>
+      <c r="W65" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7675,7 +7831,8 @@
       <c r="O66" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W66" s="1">
+      <c r="V66" s="18"/>
+      <c r="W66" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7753,7 +7910,8 @@
       <c r="O67" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W67" s="1">
+      <c r="V67" s="18"/>
+      <c r="W67" s="16">
         <f t="shared" ref="W67:W69" si="1">V67/2745186691</f>
         <v>0</v>
       </c>
@@ -7831,7 +7989,8 @@
       <c r="O68" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W68" s="1">
+      <c r="V68" s="18"/>
+      <c r="W68" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7909,7 +8068,8 @@
       <c r="O69" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W69" s="1">
+      <c r="V69" s="18"/>
+      <c r="W69" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -7987,7 +8147,8 @@
       <c r="O70" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W70" s="1">
+      <c r="V70" s="18"/>
+      <c r="W70" s="16">
         <f>V70/2745186691</f>
         <v>0</v>
       </c>
@@ -8065,7 +8226,8 @@
       <c r="O71" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W71" s="1">
+      <c r="V71" s="18"/>
+      <c r="W71" s="16">
         <f t="shared" ref="W71:W97" si="2">V71/2745186691</f>
         <v>0</v>
       </c>
@@ -8143,7 +8305,8 @@
       <c r="O72" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W72" s="1">
+      <c r="V72" s="18"/>
+      <c r="W72" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8221,7 +8384,8 @@
       <c r="O73" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W73" s="1">
+      <c r="V73" s="18"/>
+      <c r="W73" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8299,7 +8463,8 @@
       <c r="O74" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W74" s="1">
+      <c r="V74" s="18"/>
+      <c r="W74" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8377,7 +8542,8 @@
       <c r="O75" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W75" s="1">
+      <c r="V75" s="18"/>
+      <c r="W75" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8455,7 +8621,8 @@
       <c r="O76" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W76" s="1">
+      <c r="V76" s="18"/>
+      <c r="W76" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8533,7 +8700,8 @@
       <c r="O77" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W77" s="1">
+      <c r="V77" s="18"/>
+      <c r="W77" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8611,7 +8779,8 @@
       <c r="O78" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W78" s="1">
+      <c r="V78" s="18"/>
+      <c r="W78" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8689,7 +8858,8 @@
       <c r="O79" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W79" s="1">
+      <c r="V79" s="18"/>
+      <c r="W79" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8767,7 +8937,8 @@
       <c r="O80" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W80" s="1">
+      <c r="V80" s="18"/>
+      <c r="W80" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8845,7 +9016,8 @@
       <c r="O81" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W81" s="1">
+      <c r="V81" s="18"/>
+      <c r="W81" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -8923,7 +9095,8 @@
       <c r="O82" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W82" s="1">
+      <c r="V82" s="18"/>
+      <c r="W82" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9001,7 +9174,8 @@
       <c r="O83" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W83" s="1">
+      <c r="V83" s="18"/>
+      <c r="W83" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9079,7 +9253,8 @@
       <c r="O84" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W84" s="1">
+      <c r="V84" s="18"/>
+      <c r="W84" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9157,7 +9332,8 @@
       <c r="O85" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W85" s="1">
+      <c r="V85" s="18"/>
+      <c r="W85" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9235,7 +9411,8 @@
       <c r="O86" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W86" s="1">
+      <c r="V86" s="18"/>
+      <c r="W86" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9313,7 +9490,8 @@
       <c r="O87" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W87" s="1">
+      <c r="V87" s="18"/>
+      <c r="W87" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9391,7 +9569,8 @@
       <c r="O88" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W88" s="1">
+      <c r="V88" s="18"/>
+      <c r="W88" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9469,7 +9648,8 @@
       <c r="O89" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W89" s="1">
+      <c r="V89" s="18"/>
+      <c r="W89" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9547,7 +9727,8 @@
       <c r="O90" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W90" s="1">
+      <c r="V90" s="18"/>
+      <c r="W90" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9625,7 +9806,8 @@
       <c r="O91" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W91" s="1">
+      <c r="V91" s="18"/>
+      <c r="W91" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9703,7 +9885,8 @@
       <c r="O92" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W92" s="1">
+      <c r="V92" s="18"/>
+      <c r="W92" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9781,7 +9964,8 @@
       <c r="O93" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W93" s="1">
+      <c r="V93" s="18"/>
+      <c r="W93" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9859,7 +10043,8 @@
       <c r="O94" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W94" s="1">
+      <c r="V94" s="18"/>
+      <c r="W94" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -9937,7 +10122,8 @@
       <c r="O95" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W95" s="1">
+      <c r="V95" s="18"/>
+      <c r="W95" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10015,7 +10201,8 @@
       <c r="O96" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W96" s="1">
+      <c r="V96" s="18"/>
+      <c r="W96" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10093,7 +10280,8 @@
       <c r="O97" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W97" s="1">
+      <c r="V97" s="18"/>
+      <c r="W97" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10171,7 +10359,8 @@
       <c r="O98" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W98" s="1">
+      <c r="V98" s="18"/>
+      <c r="W98" s="16">
         <f>V98/2745186691</f>
         <v>0</v>
       </c>
@@ -10249,7 +10438,8 @@
       <c r="O99" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W99" s="1">
+      <c r="V99" s="18"/>
+      <c r="W99" s="16">
         <f t="shared" ref="W99:W119" si="3">V99/2745186691</f>
         <v>0</v>
       </c>
@@ -10327,7 +10517,8 @@
       <c r="O100" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W100" s="1">
+      <c r="V100" s="18"/>
+      <c r="W100" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10405,7 +10596,8 @@
       <c r="O101" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W101" s="1">
+      <c r="V101" s="18"/>
+      <c r="W101" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10483,7 +10675,8 @@
       <c r="O102" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W102" s="1">
+      <c r="V102" s="18"/>
+      <c r="W102" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10561,7 +10754,8 @@
       <c r="O103" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W103" s="1">
+      <c r="V103" s="18"/>
+      <c r="W103" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10639,7 +10833,8 @@
       <c r="O104" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W104" s="1">
+      <c r="V104" s="18"/>
+      <c r="W104" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10717,7 +10912,8 @@
       <c r="O105" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W105" s="1">
+      <c r="V105" s="18"/>
+      <c r="W105" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10795,7 +10991,8 @@
       <c r="O106" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W106" s="1">
+      <c r="V106" s="18"/>
+      <c r="W106" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10873,7 +11070,8 @@
       <c r="O107" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W107" s="1">
+      <c r="V107" s="18"/>
+      <c r="W107" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -10951,7 +11149,8 @@
       <c r="O108" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W108" s="1">
+      <c r="V108" s="18"/>
+      <c r="W108" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11029,7 +11228,8 @@
       <c r="O109" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W109" s="1">
+      <c r="V109" s="18"/>
+      <c r="W109" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11107,7 +11307,8 @@
       <c r="O110" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W110" s="1">
+      <c r="V110" s="18"/>
+      <c r="W110" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11185,7 +11386,8 @@
       <c r="O111" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W111" s="1">
+      <c r="V111" s="18"/>
+      <c r="W111" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11263,7 +11465,8 @@
       <c r="O112" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W112" s="1">
+      <c r="V112" s="18"/>
+      <c r="W112" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11341,7 +11544,8 @@
       <c r="O113" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W113" s="1">
+      <c r="V113" s="18"/>
+      <c r="W113" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11419,7 +11623,8 @@
       <c r="O114" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W114" s="1">
+      <c r="V114" s="18"/>
+      <c r="W114" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11497,7 +11702,8 @@
       <c r="O115" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W115" s="1">
+      <c r="V115" s="18"/>
+      <c r="W115" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11575,7 +11781,8 @@
       <c r="O116" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W116" s="1">
+      <c r="V116" s="18"/>
+      <c r="W116" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11653,7 +11860,8 @@
       <c r="O117" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W117" s="1">
+      <c r="V117" s="18"/>
+      <c r="W117" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11731,7 +11939,8 @@
       <c r="O118" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W118" s="1">
+      <c r="V118" s="18"/>
+      <c r="W118" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11809,7 +12018,8 @@
       <c r="O119" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W119" s="1">
+      <c r="V119" s="18"/>
+      <c r="W119" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -11887,7 +12097,8 @@
       <c r="O120" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="W120" s="1">
+      <c r="V120" s="18"/>
+      <c r="W120" s="16">
         <f>V120/2745186691</f>
         <v>0</v>
       </c>
@@ -11965,7 +12176,8 @@
       <c r="O121" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="W121" s="1">
+      <c r="V121" s="18"/>
+      <c r="W121" s="16">
         <f t="shared" ref="W121:W145" si="4">V121/2745186691</f>
         <v>0</v>
       </c>
@@ -12043,7 +12255,8 @@
       <c r="O122" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W122" s="1">
+      <c r="V122" s="18"/>
+      <c r="W122" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12121,7 +12334,8 @@
       <c r="O123" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W123" s="1">
+      <c r="V123" s="18"/>
+      <c r="W123" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12199,7 +12413,8 @@
       <c r="O124" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W124" s="1">
+      <c r="V124" s="18"/>
+      <c r="W124" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12277,7 +12492,8 @@
       <c r="O125" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W125" s="1">
+      <c r="V125" s="18"/>
+      <c r="W125" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12355,7 +12571,8 @@
       <c r="O126" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W126" s="1">
+      <c r="V126" s="18"/>
+      <c r="W126" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12433,7 +12650,8 @@
       <c r="O127" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W127" s="1">
+      <c r="V127" s="18"/>
+      <c r="W127" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12511,7 +12729,8 @@
       <c r="O128" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W128" s="1">
+      <c r="V128" s="18"/>
+      <c r="W128" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12589,7 +12808,8 @@
       <c r="O129" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W129" s="1">
+      <c r="V129" s="18"/>
+      <c r="W129" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12667,7 +12887,8 @@
       <c r="O130" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W130" s="1">
+      <c r="V130" s="18"/>
+      <c r="W130" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12745,7 +12966,8 @@
       <c r="O131" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W131" s="1">
+      <c r="V131" s="18"/>
+      <c r="W131" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12823,7 +13045,8 @@
       <c r="O132" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W132" s="1">
+      <c r="V132" s="18"/>
+      <c r="W132" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12901,7 +13124,8 @@
       <c r="O133" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W133" s="1">
+      <c r="V133" s="18"/>
+      <c r="W133" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -12979,7 +13203,8 @@
       <c r="O134" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W134" s="1">
+      <c r="V134" s="18"/>
+      <c r="W134" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13057,7 +13282,8 @@
       <c r="O135" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W135" s="1">
+      <c r="V135" s="18"/>
+      <c r="W135" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13135,7 +13361,8 @@
       <c r="O136" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W136" s="1">
+      <c r="V136" s="18"/>
+      <c r="W136" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13213,7 +13440,8 @@
       <c r="O137" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W137" s="1">
+      <c r="V137" s="18"/>
+      <c r="W137" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13291,7 +13519,8 @@
       <c r="O138" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W138" s="1">
+      <c r="V138" s="18"/>
+      <c r="W138" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13369,7 +13598,8 @@
       <c r="O139" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W139" s="1">
+      <c r="V139" s="18"/>
+      <c r="W139" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13447,7 +13677,8 @@
       <c r="O140" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W140" s="1">
+      <c r="V140" s="18"/>
+      <c r="W140" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13525,7 +13756,8 @@
       <c r="O141" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W141" s="1">
+      <c r="V141" s="18"/>
+      <c r="W141" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13603,7 +13835,8 @@
       <c r="O142" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W142" s="1">
+      <c r="V142" s="18"/>
+      <c r="W142" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13681,7 +13914,8 @@
       <c r="O143" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W143" s="1">
+      <c r="V143" s="18"/>
+      <c r="W143" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13759,7 +13993,8 @@
       <c r="O144" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W144" s="1">
+      <c r="V144" s="18"/>
+      <c r="W144" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13837,7 +14072,8 @@
       <c r="O145" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W145" s="1">
+      <c r="V145" s="18"/>
+      <c r="W145" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -13915,7 +14151,8 @@
       <c r="O146" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W146" s="1">
+      <c r="V146" s="18"/>
+      <c r="W146" s="16">
         <f>V146/2745186691</f>
         <v>0</v>
       </c>
@@ -13993,7 +14230,8 @@
       <c r="O147" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W147" s="1">
+      <c r="V147" s="18"/>
+      <c r="W147" s="16">
         <f t="shared" ref="W147:W174" si="5">V147/2745186691</f>
         <v>0</v>
       </c>
@@ -14071,7 +14309,8 @@
       <c r="O148" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W148" s="1">
+      <c r="V148" s="18"/>
+      <c r="W148" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14149,7 +14388,8 @@
       <c r="O149" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W149" s="1">
+      <c r="V149" s="18"/>
+      <c r="W149" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14227,7 +14467,8 @@
       <c r="O150" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W150" s="1">
+      <c r="V150" s="18"/>
+      <c r="W150" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14305,7 +14546,8 @@
       <c r="O151" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W151" s="1">
+      <c r="V151" s="18"/>
+      <c r="W151" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14383,7 +14625,8 @@
       <c r="O152" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W152" s="1">
+      <c r="V152" s="18"/>
+      <c r="W152" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14461,7 +14704,8 @@
       <c r="O153" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W153" s="1">
+      <c r="V153" s="18"/>
+      <c r="W153" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14539,7 +14783,8 @@
       <c r="O154" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W154" s="1">
+      <c r="V154" s="18"/>
+      <c r="W154" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14617,7 +14862,8 @@
       <c r="O155" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W155" s="1">
+      <c r="V155" s="18"/>
+      <c r="W155" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14695,7 +14941,8 @@
       <c r="O156" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W156" s="1">
+      <c r="V156" s="18"/>
+      <c r="W156" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14773,7 +15020,8 @@
       <c r="O157" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W157" s="1">
+      <c r="V157" s="18"/>
+      <c r="W157" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14851,7 +15099,8 @@
       <c r="O158" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W158" s="1">
+      <c r="V158" s="18"/>
+      <c r="W158" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -14929,7 +15178,8 @@
       <c r="O159" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W159" s="1">
+      <c r="V159" s="18"/>
+      <c r="W159" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15007,7 +15257,8 @@
       <c r="O160" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W160" s="1">
+      <c r="V160" s="18"/>
+      <c r="W160" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15085,7 +15336,8 @@
       <c r="O161" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W161" s="1">
+      <c r="V161" s="18"/>
+      <c r="W161" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15163,7 +15415,8 @@
       <c r="O162" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W162" s="1">
+      <c r="V162" s="18"/>
+      <c r="W162" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15241,7 +15494,8 @@
       <c r="O163" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W163" s="1">
+      <c r="V163" s="18"/>
+      <c r="W163" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15319,7 +15573,8 @@
       <c r="O164" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W164" s="1">
+      <c r="V164" s="18"/>
+      <c r="W164" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15397,7 +15652,8 @@
       <c r="O165" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W165" s="1">
+      <c r="V165" s="18"/>
+      <c r="W165" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15475,7 +15731,8 @@
       <c r="O166" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W166" s="1">
+      <c r="V166" s="18"/>
+      <c r="W166" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15553,7 +15810,8 @@
       <c r="O167" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W167" s="1">
+      <c r="V167" s="18"/>
+      <c r="W167" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15631,7 +15889,8 @@
       <c r="O168" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W168" s="1">
+      <c r="V168" s="18"/>
+      <c r="W168" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15709,7 +15968,8 @@
       <c r="O169" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W169" s="1">
+      <c r="V169" s="18"/>
+      <c r="W169" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15787,7 +16047,8 @@
       <c r="O170" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W170" s="1">
+      <c r="V170" s="18"/>
+      <c r="W170" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15865,7 +16126,8 @@
       <c r="O171" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W171" s="1">
+      <c r="V171" s="18"/>
+      <c r="W171" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -15943,7 +16205,8 @@
       <c r="O172" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W172" s="1">
+      <c r="V172" s="18"/>
+      <c r="W172" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -16021,7 +16284,8 @@
       <c r="O173" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W173" s="1">
+      <c r="V173" s="18"/>
+      <c r="W173" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -16099,7 +16363,8 @@
       <c r="O174" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W174" s="1">
+      <c r="V174" s="18"/>
+      <c r="W174" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -16177,7 +16442,8 @@
       <c r="O175" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W175" s="1">
+      <c r="V175" s="18"/>
+      <c r="W175" s="16">
         <f>V175/2745186691</f>
         <v>0</v>
       </c>
@@ -16255,7 +16521,8 @@
       <c r="O176" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W176" s="1">
+      <c r="V176" s="18"/>
+      <c r="W176" s="16">
         <f t="shared" ref="W176:W203" si="6">V176/2745186691</f>
         <v>0</v>
       </c>
@@ -16333,7 +16600,8 @@
       <c r="O177" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W177" s="1">
+      <c r="V177" s="18"/>
+      <c r="W177" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -16411,7 +16679,8 @@
       <c r="O178" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W178" s="1">
+      <c r="V178" s="18"/>
+      <c r="W178" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -16489,7 +16758,8 @@
       <c r="O179" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W179" s="1">
+      <c r="V179" s="18"/>
+      <c r="W179" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -16567,7 +16837,8 @@
       <c r="O180" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W180" s="1">
+      <c r="V180" s="18"/>
+      <c r="W180" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -16645,7 +16916,8 @@
       <c r="O181" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W181" s="1">
+      <c r="V181" s="18"/>
+      <c r="W181" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -16723,7 +16995,8 @@
       <c r="O182" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W182" s="1">
+      <c r="V182" s="18"/>
+      <c r="W182" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -16801,7 +17074,8 @@
       <c r="O183" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W183" s="1">
+      <c r="V183" s="18"/>
+      <c r="W183" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -16879,7 +17153,8 @@
       <c r="O184" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W184" s="1">
+      <c r="V184" s="18"/>
+      <c r="W184" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -16957,7 +17232,8 @@
       <c r="O185" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W185" s="1">
+      <c r="V185" s="18"/>
+      <c r="W185" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17035,7 +17311,8 @@
       <c r="O186" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W186" s="1">
+      <c r="V186" s="18"/>
+      <c r="W186" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17113,7 +17390,8 @@
       <c r="O187" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W187" s="1">
+      <c r="V187" s="18"/>
+      <c r="W187" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17191,7 +17469,8 @@
       <c r="O188" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W188" s="1">
+      <c r="V188" s="18"/>
+      <c r="W188" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17269,7 +17548,8 @@
       <c r="O189" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W189" s="1">
+      <c r="V189" s="18"/>
+      <c r="W189" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17347,7 +17627,8 @@
       <c r="O190" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W190" s="1">
+      <c r="V190" s="18"/>
+      <c r="W190" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17425,7 +17706,8 @@
       <c r="O191" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W191" s="1">
+      <c r="V191" s="18"/>
+      <c r="W191" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17503,7 +17785,8 @@
       <c r="O192" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W192" s="1">
+      <c r="V192" s="18"/>
+      <c r="W192" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17581,7 +17864,8 @@
       <c r="O193" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W193" s="1">
+      <c r="V193" s="18"/>
+      <c r="W193" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17659,7 +17943,8 @@
       <c r="O194" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W194" s="1">
+      <c r="V194" s="18"/>
+      <c r="W194" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17737,7 +18022,8 @@
       <c r="O195" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W195" s="1">
+      <c r="V195" s="18"/>
+      <c r="W195" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17815,7 +18101,8 @@
       <c r="O196" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W196" s="1">
+      <c r="V196" s="18"/>
+      <c r="W196" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17893,7 +18180,8 @@
       <c r="O197" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W197" s="1">
+      <c r="V197" s="18"/>
+      <c r="W197" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17971,7 +18259,8 @@
       <c r="O198" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W198" s="1">
+      <c r="V198" s="18"/>
+      <c r="W198" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -18049,7 +18338,8 @@
       <c r="O199" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="W199" s="1">
+      <c r="V199" s="18"/>
+      <c r="W199" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -18127,7 +18417,8 @@
       <c r="O200" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="W200" s="1">
+      <c r="V200" s="18"/>
+      <c r="W200" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -18211,6 +18502,9 @@
       <c r="Q201" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R201" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S201" s="14">
         <v>0.95318800000000004</v>
       </c>
@@ -18220,10 +18514,10 @@
       <c r="U201" s="14">
         <v>12.337153000000001</v>
       </c>
-      <c r="V201" s="1">
+      <c r="V201" s="18">
         <v>2016158349</v>
       </c>
-      <c r="W201" s="1">
+      <c r="W201" s="16">
         <f t="shared" si="6"/>
         <v>0.73443396604314948</v>
       </c>
@@ -18308,6 +18602,9 @@
       <c r="Q202" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R202" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S202" s="14">
         <v>0.96416500000000005</v>
       </c>
@@ -18317,10 +18614,10 @@
       <c r="U202" s="14">
         <v>11.501649</v>
       </c>
-      <c r="V202" s="1">
+      <c r="V202" s="18">
         <v>1999813870</v>
       </c>
-      <c r="W202" s="1">
+      <c r="W202" s="16">
         <f t="shared" si="6"/>
         <v>0.72848009811366232</v>
       </c>
@@ -18405,6 +18702,9 @@
       <c r="Q203" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R203" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S203" s="14">
         <v>0.95740099999999995</v>
       </c>
@@ -18414,10 +18714,10 @@
       <c r="U203" s="14">
         <v>12.405120999999999</v>
       </c>
-      <c r="V203" s="1">
+      <c r="V203" s="18">
         <v>2026204717</v>
       </c>
-      <c r="W203" s="1">
+      <c r="W203" s="16">
         <f t="shared" si="6"/>
         <v>0.73809359619979298</v>
       </c>
@@ -18502,6 +18802,9 @@
       <c r="Q204" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R204" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S204" s="14">
         <v>0.969692</v>
       </c>
@@ -18511,10 +18814,10 @@
       <c r="U204" s="14">
         <v>12.356994</v>
       </c>
-      <c r="V204" s="1">
+      <c r="V204" s="18">
         <v>2113763418</v>
       </c>
-      <c r="W204" s="1">
+      <c r="W204" s="16">
         <f>V204/2745186691</f>
         <v>0.76998895008849511</v>
       </c>
@@ -18599,6 +18902,9 @@
       <c r="Q205" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R205" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S205" s="14">
         <v>0.969032</v>
       </c>
@@ -18608,10 +18914,10 @@
       <c r="U205" s="14">
         <v>12.620317</v>
       </c>
-      <c r="V205" s="1">
+      <c r="V205" s="18">
         <v>2128109523</v>
       </c>
-      <c r="W205" s="1">
+      <c r="W205" s="16">
         <f>V205/2745186691</f>
         <v>0.77521486242700133</v>
       </c>
@@ -18696,6 +19002,9 @@
       <c r="Q206" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R206" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S206" s="14">
         <v>0.96321800000000002</v>
       </c>
@@ -18705,10 +19014,10 @@
       <c r="U206" s="14">
         <v>14.008304000000001</v>
       </c>
-      <c r="V206" s="1">
+      <c r="V206" s="18">
         <v>2070915893</v>
       </c>
-      <c r="W206" s="1">
+      <c r="W206" s="16">
         <f t="shared" ref="W206:W237" si="7">V206/2745186691</f>
         <v>0.75438071289993736</v>
       </c>
@@ -18766,6 +19075,9 @@
       <c r="Q207" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R207" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S207" s="14">
         <v>0.96457000000000004</v>
       </c>
@@ -18775,10 +19087,10 @@
       <c r="U207" s="14">
         <v>15.552664999999999</v>
       </c>
-      <c r="V207" s="1">
+      <c r="V207" s="18">
         <v>2157056738</v>
       </c>
-      <c r="W207" s="1">
+      <c r="W207" s="16">
         <f t="shared" si="7"/>
         <v>0.78575957878268765</v>
       </c>
@@ -18836,6 +19148,9 @@
       <c r="Q208" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R208" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S208" s="14">
         <v>0.96468900000000002</v>
       </c>
@@ -18845,10 +19160,10 @@
       <c r="U208" s="14">
         <v>13.209941000000001</v>
       </c>
-      <c r="V208" s="1">
+      <c r="V208" s="18">
         <v>2083836930</v>
       </c>
-      <c r="W208" s="1">
+      <c r="W208" s="16">
         <f t="shared" si="7"/>
         <v>0.75908751008876285</v>
       </c>
@@ -18906,6 +19221,9 @@
       <c r="Q209" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R209" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S209" s="14">
         <v>0.96056699999999995</v>
       </c>
@@ -18915,10 +19233,10 @@
       <c r="U209" s="14">
         <v>13.502068</v>
       </c>
-      <c r="V209" s="1">
+      <c r="V209" s="18">
         <v>2016920453</v>
       </c>
-      <c r="W209" s="1">
+      <c r="W209" s="16">
         <f t="shared" si="7"/>
         <v>0.73471158067770193</v>
       </c>
@@ -18976,6 +19294,9 @@
       <c r="Q210" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R210" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S210" s="14">
         <v>0.96444099999999999</v>
       </c>
@@ -18985,10 +19306,10 @@
       <c r="U210" s="14">
         <v>14.183344999999999</v>
       </c>
-      <c r="V210" s="1">
+      <c r="V210" s="18">
         <v>2102748179</v>
       </c>
-      <c r="W210" s="1">
+      <c r="W210" s="16">
         <f t="shared" si="7"/>
         <v>0.76597638546543578</v>
       </c>
@@ -19046,6 +19367,9 @@
       <c r="Q211" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R211" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S211" s="14">
         <v>0.95903300000000002</v>
       </c>
@@ -19055,10 +19379,10 @@
       <c r="U211" s="14">
         <v>13.029605999999999</v>
       </c>
-      <c r="V211" s="1">
+      <c r="V211" s="18">
         <v>1965729537</v>
       </c>
-      <c r="W211" s="1">
+      <c r="W211" s="16">
         <f t="shared" si="7"/>
         <v>0.71606406349141083</v>
       </c>
@@ -19116,6 +19440,9 @@
       <c r="Q212" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R212" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S212" s="14">
         <v>0.96003499999999997</v>
       </c>
@@ -19125,10 +19452,10 @@
       <c r="U212" s="14">
         <v>12.078849</v>
       </c>
-      <c r="V212" s="1">
+      <c r="V212" s="18">
         <v>1958252633</v>
       </c>
-      <c r="W212" s="1">
+      <c r="W212" s="16">
         <f t="shared" si="7"/>
         <v>0.71334042213597482</v>
       </c>
@@ -19186,6 +19513,9 @@
       <c r="Q213" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R213" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S213" s="14">
         <v>0.96581399999999995</v>
       </c>
@@ -19195,10 +19525,10 @@
       <c r="U213" s="14">
         <v>15.951718</v>
       </c>
-      <c r="V213" s="1">
+      <c r="V213" s="18">
         <v>2203574473</v>
       </c>
-      <c r="W213" s="1">
+      <c r="W213" s="16">
         <f t="shared" si="7"/>
         <v>0.80270477786605299</v>
       </c>
@@ -19256,6 +19586,9 @@
       <c r="Q214" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="R214" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S214" s="14">
         <v>0.97803200000000001</v>
       </c>
@@ -19265,10 +19598,10 @@
       <c r="U214" s="14">
         <v>26.182586000000001</v>
       </c>
-      <c r="V214" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="W214" s="1" t="e">
+      <c r="V214" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="W214" s="16" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
@@ -19352,6 +19685,9 @@
       <c r="Q215" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="R215" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S215" s="14">
         <v>0.97728700000000002</v>
       </c>
@@ -19361,10 +19697,10 @@
       <c r="U215" s="14">
         <v>28.024922</v>
       </c>
-      <c r="V215" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="W215" s="1" t="e">
+      <c r="V215" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="W215" s="16" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
@@ -19448,6 +19784,9 @@
       <c r="Q216" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R216" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S216" s="13">
         <v>0.89538300000000004</v>
       </c>
@@ -19457,10 +19796,10 @@
       <c r="U216" s="15">
         <v>8.713984</v>
       </c>
-      <c r="V216" s="1">
+      <c r="V216" s="18">
         <v>1313388880</v>
       </c>
-      <c r="W216" s="1">
+      <c r="W216" s="16">
         <f t="shared" si="7"/>
         <v>0.47843335548212446</v>
       </c>
@@ -19517,6 +19856,9 @@
       <c r="Q217" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R217" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S217" s="13">
         <v>0.95650900000000005</v>
       </c>
@@ -19526,10 +19868,10 @@
       <c r="U217" s="15">
         <v>8.6951210000000003</v>
       </c>
-      <c r="V217" s="1">
+      <c r="V217" s="18">
         <v>1519346612</v>
       </c>
-      <c r="W217" s="1">
+      <c r="W217" s="16">
         <f t="shared" si="7"/>
         <v>0.55345839209447045</v>
       </c>
@@ -19613,6 +19955,9 @@
       <c r="Q218" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R218" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S218" s="13">
         <v>0.91670099999999999</v>
       </c>
@@ -19622,10 +19967,10 @@
       <c r="U218" s="15">
         <v>9.7677359999999993</v>
       </c>
-      <c r="V218" s="1">
+      <c r="V218" s="18">
         <v>1496672757</v>
       </c>
-      <c r="W218" s="1">
+      <c r="W218" s="16">
         <f t="shared" si="7"/>
         <v>0.54519889736708615</v>
       </c>
@@ -19709,6 +20054,9 @@
       <c r="Q219" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R219" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S219" s="1">
         <v>0.94728400000000001</v>
       </c>
@@ -19718,10 +20066,10 @@
       <c r="U219" s="14">
         <v>8.1514520000000008</v>
       </c>
-      <c r="V219" s="1">
+      <c r="V219" s="18">
         <v>1397397283</v>
       </c>
-      <c r="W219" s="1">
+      <c r="W219" s="16">
         <f t="shared" si="7"/>
         <v>0.50903542829393678</v>
       </c>
@@ -19805,6 +20153,9 @@
       <c r="Q220" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R220" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S220" s="1">
         <v>0.96030199999999999</v>
       </c>
@@ -19814,10 +20165,10 @@
       <c r="U220" s="14">
         <v>12.101818</v>
       </c>
-      <c r="V220" s="1">
+      <c r="V220" s="18">
         <v>2017196710</v>
       </c>
-      <c r="W220" s="1">
+      <c r="W220" s="16">
         <f t="shared" si="7"/>
         <v>0.73481221390636564</v>
       </c>
@@ -19901,6 +20252,9 @@
       <c r="Q221" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R221" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S221" s="14">
         <v>0.96584099999999995</v>
       </c>
@@ -19910,10 +20264,10 @@
       <c r="U221" s="14">
         <v>15.672454</v>
       </c>
-      <c r="V221" s="13">
+      <c r="V221" s="17">
         <v>2135615082</v>
       </c>
-      <c r="W221" s="1">
+      <c r="W221" s="16">
         <f t="shared" si="7"/>
         <v>0.77794894205248066</v>
       </c>
@@ -19971,6 +20325,9 @@
       <c r="Q222" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R222" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S222" s="14">
         <v>0.96598300000000004</v>
       </c>
@@ -19980,10 +20337,10 @@
       <c r="U222" s="14">
         <v>17.521547999999999</v>
       </c>
-      <c r="V222" s="13">
+      <c r="V222" s="17">
         <v>2245997406</v>
       </c>
-      <c r="W222" s="1">
+      <c r="W222" s="16">
         <f t="shared" si="7"/>
         <v>0.81815834724954228</v>
       </c>
@@ -20041,6 +20398,9 @@
       <c r="Q223" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R223" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S223" s="14">
         <v>0.929199</v>
       </c>
@@ -20050,10 +20410,10 @@
       <c r="U223" s="14">
         <v>17.568660999999999</v>
       </c>
-      <c r="V223" s="13">
+      <c r="V223" s="17">
         <v>2008333582</v>
       </c>
-      <c r="W223" s="1">
+      <c r="W223" s="16">
         <f t="shared" si="7"/>
         <v>0.73158360725857097</v>
       </c>
@@ -20111,6 +20471,9 @@
       <c r="Q224" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R224" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S224" s="14">
         <v>0.93560299999999996</v>
       </c>
@@ -20120,10 +20483,10 @@
       <c r="U224" s="14">
         <v>14.093051000000001</v>
       </c>
-      <c r="V224" s="13">
+      <c r="V224" s="17">
         <v>1896721398</v>
       </c>
-      <c r="W224" s="1">
+      <c r="W224" s="16">
         <f t="shared" si="7"/>
         <v>0.69092619610110151</v>
       </c>
@@ -20181,6 +20544,9 @@
       <c r="Q225" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R225" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S225" s="14">
         <v>0.96881499999999998</v>
       </c>
@@ -20190,10 +20556,10 @@
       <c r="U225" s="14">
         <v>17.778409</v>
       </c>
-      <c r="V225" s="13">
+      <c r="V225" s="17">
         <v>2289354297</v>
       </c>
-      <c r="W225" s="1">
+      <c r="W225" s="16">
         <f t="shared" si="7"/>
         <v>0.83395213320302375</v>
       </c>
@@ -20251,6 +20617,9 @@
       <c r="Q226" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R226" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S226" s="14">
         <v>0.87577199999999999</v>
       </c>
@@ -20260,10 +20629,10 @@
       <c r="U226" s="14">
         <v>16.852029999999999</v>
       </c>
-      <c r="V226" s="13">
+      <c r="V226" s="17">
         <v>1852656898</v>
       </c>
-      <c r="W226" s="1">
+      <c r="W226" s="16">
         <f t="shared" si="7"/>
         <v>0.67487464662198449</v>
       </c>
@@ -20321,6 +20690,9 @@
       <c r="Q227" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R227" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S227" s="14">
         <v>0.89684799999999998</v>
       </c>
@@ -20330,10 +20702,10 @@
       <c r="U227" s="14">
         <v>15.712006000000001</v>
       </c>
-      <c r="V227" s="13">
+      <c r="V227" s="17">
         <v>1861074375</v>
       </c>
-      <c r="W227" s="1">
+      <c r="W227" s="16">
         <f t="shared" si="7"/>
         <v>0.67794091421959324</v>
       </c>
@@ -20391,6 +20763,9 @@
       <c r="Q228" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R228" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S228" s="14">
         <v>0.81608199999999997</v>
       </c>
@@ -20400,10 +20775,10 @@
       <c r="U228" s="14">
         <v>18.739588999999999</v>
       </c>
-      <c r="V228" s="13">
+      <c r="V228" s="17">
         <v>1776282370</v>
       </c>
-      <c r="W228" s="1">
+      <c r="W228" s="16">
         <f t="shared" si="7"/>
         <v>0.64705339561184694</v>
       </c>
@@ -20461,6 +20836,9 @@
       <c r="Q229" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R229" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S229" s="14">
         <v>0.96493700000000004</v>
       </c>
@@ -20470,10 +20848,10 @@
       <c r="U229" s="14">
         <v>16.990945</v>
       </c>
-      <c r="V229" s="13">
+      <c r="V229" s="17">
         <v>2181551544</v>
       </c>
-      <c r="W229" s="1">
+      <c r="W229" s="16">
         <f t="shared" si="7"/>
         <v>0.79468239852398437</v>
       </c>
@@ -20531,6 +20909,9 @@
       <c r="Q230" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R230" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S230" s="14">
         <v>0.97229100000000002</v>
       </c>
@@ -20540,10 +20921,10 @@
       <c r="U230" s="14">
         <v>24.633641000000001</v>
       </c>
-      <c r="V230" s="13">
+      <c r="V230" s="17">
         <v>2407179313</v>
       </c>
-      <c r="W230" s="1">
+      <c r="W230" s="16">
         <f t="shared" si="7"/>
         <v>0.87687271721513671</v>
       </c>
@@ -20601,6 +20982,9 @@
       <c r="Q231" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R231" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S231" s="14">
         <v>0.96257300000000001</v>
       </c>
@@ -20610,10 +20994,10 @@
       <c r="U231" s="14">
         <v>17.425408999999998</v>
       </c>
-      <c r="V231" s="13">
+      <c r="V231" s="17">
         <v>2190016898</v>
       </c>
-      <c r="W231" s="1">
+      <c r="W231" s="16">
         <f t="shared" si="7"/>
         <v>0.79776610646550739</v>
       </c>
@@ -20671,6 +21055,9 @@
       <c r="Q232" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R232" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S232" s="14">
         <v>0.962696</v>
       </c>
@@ -20680,10 +21067,10 @@
       <c r="U232" s="14">
         <v>18.71536</v>
       </c>
-      <c r="V232" s="13">
+      <c r="V232" s="17">
         <v>2223630318</v>
       </c>
-      <c r="W232" s="1">
+      <c r="W232" s="16">
         <f t="shared" si="7"/>
         <v>0.81001059974904277</v>
       </c>
@@ -20741,6 +21128,9 @@
       <c r="Q233" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="R233" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S233" s="14">
         <v>0.97843999999999998</v>
       </c>
@@ -20750,10 +21140,10 @@
       <c r="U233" s="14">
         <v>38.064106000000002</v>
       </c>
-      <c r="V233" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="W233" s="1" t="e">
+      <c r="V233" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="W233" s="16" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
@@ -20837,6 +21227,9 @@
       <c r="Q234" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R234" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S234" s="13">
         <v>0.90837400000000001</v>
       </c>
@@ -20846,10 +21239,10 @@
       <c r="U234" s="15">
         <v>10.786854999999999</v>
       </c>
-      <c r="V234" s="13">
+      <c r="V234" s="17">
         <v>1680818187</v>
       </c>
-      <c r="W234" s="1">
+      <c r="W234" s="16">
         <f>V234/2745186691</f>
         <v>0.61227828056667499</v>
       </c>
@@ -20906,6 +21299,9 @@
       <c r="Q235" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R235" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S235" s="13">
         <v>0.87366100000000002</v>
       </c>
@@ -20915,10 +21311,10 @@
       <c r="U235" s="15">
         <v>11.180037</v>
       </c>
-      <c r="V235" s="13">
+      <c r="V235" s="17">
         <v>1591351615</v>
       </c>
-      <c r="W235" s="1">
+      <c r="W235" s="16">
         <f t="shared" si="7"/>
         <v>0.57968793897230797</v>
       </c>
@@ -20975,6 +21371,9 @@
       <c r="Q236" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R236" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S236" s="13">
         <v>0.87476900000000002</v>
       </c>
@@ -20984,10 +21383,10 @@
       <c r="U236" s="15">
         <v>9.4556979999999999</v>
       </c>
-      <c r="V236" s="13">
+      <c r="V236" s="17">
         <v>1420378243</v>
       </c>
-      <c r="W236" s="1">
+      <c r="W236" s="16">
         <f t="shared" si="7"/>
         <v>0.51740679337280093</v>
       </c>
@@ -21044,6 +21443,9 @@
       <c r="Q237" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R237" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S237" s="13">
         <v>0.90007400000000004</v>
       </c>
@@ -21053,10 +21455,10 @@
       <c r="U237" s="15">
         <v>8.0067810000000001</v>
       </c>
-      <c r="V237" s="13">
+      <c r="V237" s="17">
         <v>1318711991</v>
       </c>
-      <c r="W237" s="1">
+      <c r="W237" s="16">
         <f t="shared" si="7"/>
         <v>0.48037242615351144</v>
       </c>
@@ -21113,6 +21515,9 @@
       <c r="Q238" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R238" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S238" s="13">
         <v>0.904914</v>
       </c>
@@ -21122,10 +21527,10 @@
       <c r="U238" s="15">
         <v>8.9634719999999994</v>
       </c>
-      <c r="V238" s="13">
+      <c r="V238" s="17">
         <v>1499602707</v>
       </c>
-      <c r="W238" s="1">
+      <c r="W238" s="16">
         <f>V238/2745186691</f>
         <v>0.54626620182750985</v>
       </c>
@@ -21182,6 +21587,9 @@
       <c r="Q239" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R239" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S239" s="13">
         <v>0.939307</v>
       </c>
@@ -21191,10 +21599,10 @@
       <c r="U239" s="15">
         <v>10.58568</v>
       </c>
-      <c r="V239" s="13">
+      <c r="V239" s="17">
         <v>1739156010</v>
       </c>
-      <c r="W239" s="1">
+      <c r="W239" s="16">
         <f t="shared" ref="W239:W261" si="8">V239/2745186691</f>
         <v>0.63352922979765391</v>
       </c>
@@ -21251,6 +21659,9 @@
       <c r="Q240" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R240" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S240" s="13">
         <v>0.94738199999999995</v>
       </c>
@@ -21260,10 +21671,10 @@
       <c r="U240" s="15">
         <v>24.572139</v>
       </c>
-      <c r="V240" s="13">
+      <c r="V240" s="17">
         <v>2286507578</v>
       </c>
-      <c r="W240" s="1">
+      <c r="W240" s="16">
         <f t="shared" si="8"/>
         <v>0.83291514762775021</v>
       </c>
@@ -21320,6 +21731,9 @@
       <c r="Q241" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R241" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S241" s="13">
         <v>0.95097100000000001</v>
       </c>
@@ -21329,10 +21743,10 @@
       <c r="U241" s="15">
         <v>9.0070270000000008</v>
       </c>
-      <c r="V241" s="13">
+      <c r="V241" s="17">
         <v>1608950839</v>
       </c>
-      <c r="W241" s="1">
+      <c r="W241" s="16">
         <f t="shared" si="8"/>
         <v>0.58609887781945391</v>
       </c>
@@ -21389,6 +21803,9 @@
       <c r="Q242" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R242" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S242" s="13">
         <v>0.89761299999999999</v>
       </c>
@@ -21398,10 +21815,10 @@
       <c r="U242" s="15">
         <v>11.459695999999999</v>
       </c>
-      <c r="V242" s="13">
+      <c r="V242" s="17">
         <v>1688812152</v>
       </c>
-      <c r="W242" s="1">
+      <c r="W242" s="16">
         <f t="shared" si="8"/>
         <v>0.61519027377508151</v>
       </c>
@@ -21458,6 +21875,9 @@
       <c r="Q243" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R243" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S243" s="14">
         <v>0.97045899999999996</v>
       </c>
@@ -21467,10 +21887,10 @@
       <c r="U243" s="14">
         <v>22.049592000000001</v>
       </c>
-      <c r="V243" s="13">
+      <c r="V243" s="17">
         <v>2336493955</v>
       </c>
-      <c r="W243" s="1">
+      <c r="W243" s="16">
         <f t="shared" si="8"/>
         <v>0.85112388263432681</v>
       </c>
@@ -21528,6 +21948,9 @@
       <c r="Q244" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R244" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S244" s="14">
         <v>0.96103799999999995</v>
       </c>
@@ -21537,10 +21960,10 @@
       <c r="U244" s="14">
         <v>16.687987</v>
       </c>
-      <c r="V244" s="13">
+      <c r="V244" s="17">
         <v>2135158011</v>
       </c>
-      <c r="W244" s="1">
+      <c r="W244" s="16">
         <f t="shared" si="8"/>
         <v>0.7777824429937833</v>
       </c>
@@ -21598,6 +22021,9 @@
       <c r="Q245" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R245" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S245" s="14">
         <v>0.97346200000000005</v>
       </c>
@@ -21607,10 +22033,10 @@
       <c r="U245" s="14">
         <v>17.728159000000002</v>
       </c>
-      <c r="V245" s="13">
+      <c r="V245" s="17">
         <v>2352933740</v>
       </c>
-      <c r="W245" s="1">
+      <c r="W245" s="16">
         <f t="shared" si="8"/>
         <v>0.85711246805691288</v>
       </c>
@@ -21668,6 +22094,9 @@
       <c r="Q246" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R246" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S246" s="14">
         <v>0.96896499999999997</v>
       </c>
@@ -21677,10 +22106,10 @@
       <c r="U246" s="14">
         <v>17.060396999999998</v>
       </c>
-      <c r="V246" s="13">
+      <c r="V246" s="17">
         <v>2212990732</v>
       </c>
-      <c r="W246" s="1">
+      <c r="W246" s="16">
         <f t="shared" si="8"/>
         <v>0.8061348757282023</v>
       </c>
@@ -21738,6 +22167,9 @@
       <c r="Q247" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R247" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S247" s="14">
         <v>0.96991799999999995</v>
       </c>
@@ -21747,10 +22179,10 @@
       <c r="U247" s="14">
         <v>17.526340000000001</v>
       </c>
-      <c r="V247" s="13">
+      <c r="V247" s="17">
         <v>2264330254</v>
       </c>
-      <c r="W247" s="1">
+      <c r="W247" s="16">
         <f t="shared" si="8"/>
         <v>0.82483652620913861</v>
       </c>
@@ -21808,6 +22240,9 @@
       <c r="Q248" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R248" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S248" s="14">
         <v>0.96834500000000001</v>
       </c>
@@ -21817,10 +22252,10 @@
       <c r="U248" s="14">
         <v>18.282527999999999</v>
       </c>
-      <c r="V248" s="13">
+      <c r="V248" s="17">
         <v>2254105304</v>
       </c>
-      <c r="W248" s="1">
+      <c r="W248" s="16">
         <f t="shared" si="8"/>
         <v>0.82111184328191833</v>
       </c>
@@ -21878,6 +22313,9 @@
       <c r="Q249" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R249" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S249" s="14">
         <v>0.97102699999999997</v>
       </c>
@@ -21887,10 +22325,10 @@
       <c r="U249" s="14">
         <v>18.133797000000001</v>
       </c>
-      <c r="V249" s="13">
+      <c r="V249" s="17">
         <v>2294595372</v>
       </c>
-      <c r="W249" s="1">
+      <c r="W249" s="16">
         <f t="shared" si="8"/>
         <v>0.83586132029663118</v>
       </c>
@@ -21948,6 +22386,9 @@
       <c r="Q250" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R250" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S250" s="14">
         <v>0.97300299999999995</v>
       </c>
@@ -21957,10 +22398,10 @@
       <c r="U250" s="14">
         <v>23.246834</v>
       </c>
-      <c r="V250" s="13">
+      <c r="V250" s="17">
         <v>2407613352</v>
       </c>
-      <c r="W250" s="1">
+      <c r="W250" s="16">
         <f t="shared" si="8"/>
         <v>0.87703082631621287</v>
       </c>
@@ -22018,6 +22459,9 @@
       <c r="Q251" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R251" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S251" s="14">
         <v>0.96191300000000002</v>
       </c>
@@ -22027,10 +22471,10 @@
       <c r="U251" s="14">
         <v>17.168365999999999</v>
       </c>
-      <c r="V251" s="13">
+      <c r="V251" s="17">
         <v>2163373885</v>
       </c>
-      <c r="W251" s="1">
+      <c r="W251" s="16">
         <f t="shared" si="8"/>
         <v>0.78806075087444749</v>
       </c>
@@ -22088,6 +22532,9 @@
       <c r="Q252" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R252" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S252" s="14">
         <v>0.956592</v>
       </c>
@@ -22097,10 +22544,10 @@
       <c r="U252" s="14">
         <v>22.387366</v>
       </c>
-      <c r="V252" s="13">
+      <c r="V252" s="17">
         <v>2213386194</v>
       </c>
-      <c r="W252" s="1">
+      <c r="W252" s="16">
         <f t="shared" si="8"/>
         <v>0.8062789322331011</v>
       </c>
@@ -22158,6 +22605,9 @@
       <c r="Q253" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R253" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S253" s="14">
         <v>0.96987000000000001</v>
       </c>
@@ -22167,10 +22617,10 @@
       <c r="U253" s="14">
         <v>21.240024999999999</v>
       </c>
-      <c r="V253" s="13">
+      <c r="V253" s="17">
         <v>2309351750</v>
       </c>
-      <c r="W253" s="1">
+      <c r="W253" s="16">
         <f t="shared" si="8"/>
         <v>0.84123668440151267</v>
       </c>
@@ -22228,6 +22678,9 @@
       <c r="Q254" s="1" t="s">
         <v>421</v>
       </c>
+      <c r="R254" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S254" s="14">
         <v>0.95205399999999996</v>
       </c>
@@ -22237,10 +22690,10 @@
       <c r="U254" s="14">
         <v>16.893682999999999</v>
       </c>
-      <c r="V254" s="13">
+      <c r="V254" s="17">
         <v>2063669340</v>
       </c>
-      <c r="W254" s="1">
+      <c r="W254" s="16">
         <f t="shared" si="8"/>
         <v>0.75174098241320664</v>
       </c>
@@ -22298,6 +22751,9 @@
       <c r="Q255" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="R255" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S255" s="14">
         <v>0.97810200000000003</v>
       </c>
@@ -22307,10 +22763,10 @@
       <c r="U255" s="14">
         <v>31.707049999999999</v>
       </c>
-      <c r="V255" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="W255" s="1" t="e">
+      <c r="V255" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="W255" s="16" t="e">
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
@@ -22379,6 +22835,9 @@
       <c r="Q256" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="R256" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="S256" s="14">
         <v>0.97805399999999998</v>
       </c>
@@ -22388,10 +22847,10 @@
       <c r="U256" s="14">
         <v>30.163716999999998</v>
       </c>
-      <c r="V256" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="W256" s="1" t="e">
+      <c r="V256" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="W256" s="16" t="e">
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
@@ -22448,6 +22907,9 @@
       <c r="Q257" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R257" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S257" s="1">
         <v>0.95584100000000005</v>
       </c>
@@ -22457,10 +22919,10 @@
       <c r="U257" s="14">
         <v>8.9852270000000001</v>
       </c>
-      <c r="V257" s="13">
+      <c r="V257" s="17">
         <v>1541526462</v>
       </c>
-      <c r="W257" s="1">
+      <c r="W257" s="16">
         <f t="shared" si="8"/>
         <v>0.56153793366908034</v>
       </c>
@@ -22517,6 +22979,9 @@
       <c r="Q258" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R258" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S258" s="1">
         <v>0.947299</v>
       </c>
@@ -22526,10 +22991,10 @@
       <c r="U258" s="14">
         <v>7.6061680000000003</v>
       </c>
-      <c r="V258" s="13">
+      <c r="V258" s="17">
         <v>1262504338</v>
       </c>
-      <c r="W258" s="1">
+      <c r="W258" s="16">
         <f t="shared" si="8"/>
         <v>0.45989744236305569</v>
       </c>
@@ -22586,6 +23051,9 @@
       <c r="Q259" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R259" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S259" s="1">
         <v>0.95092900000000002</v>
       </c>
@@ -22595,10 +23063,10 @@
       <c r="U259" s="14">
         <v>10.018302</v>
       </c>
-      <c r="V259" s="13">
+      <c r="V259" s="17">
         <v>1650869775</v>
       </c>
-      <c r="W259" s="1">
+      <c r="W259" s="16">
         <f t="shared" si="8"/>
         <v>0.60136885422485831</v>
       </c>
@@ -22655,6 +23123,9 @@
       <c r="Q260" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R260" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S260" s="1">
         <v>0.96204000000000001</v>
       </c>
@@ -22664,10 +23135,10 @@
       <c r="U260" s="14">
         <v>11.199862</v>
       </c>
-      <c r="V260" s="13">
+      <c r="V260" s="17">
         <v>1900700497</v>
       </c>
-      <c r="W260" s="1">
+      <c r="W260" s="16">
         <f t="shared" si="8"/>
         <v>0.69237567821211621</v>
       </c>
@@ -22724,6 +23195,9 @@
       <c r="Q261" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R261" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S261" s="1">
         <v>0.950353</v>
       </c>
@@ -22733,10 +23207,10 @@
       <c r="U261" s="14">
         <v>8.6108440000000002</v>
       </c>
-      <c r="V261" s="13">
+      <c r="V261" s="17">
         <v>1445894095</v>
       </c>
-      <c r="W261" s="1">
+      <c r="W261" s="16">
         <f t="shared" si="8"/>
         <v>0.52670155357386583</v>
       </c>
@@ -22793,6 +23267,9 @@
       <c r="Q262" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R262" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S262" s="1">
         <v>0.94986400000000004</v>
       </c>
@@ -22802,10 +23279,10 @@
       <c r="U262" s="14">
         <v>8.9786350000000006</v>
       </c>
-      <c r="V262" s="13">
+      <c r="V262" s="17">
         <v>1504838317</v>
       </c>
-      <c r="W262" s="1">
+      <c r="W262" s="16">
         <f>V262/2745186691</f>
         <v>0.54817339816397936</v>
       </c>
@@ -22862,6 +23339,9 @@
       <c r="Q263" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R263" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S263" s="1">
         <v>0.945739</v>
       </c>
@@ -22871,10 +23351,10 @@
       <c r="U263" s="14">
         <v>9.2027380000000001</v>
       </c>
-      <c r="V263" s="13">
+      <c r="V263" s="17">
         <v>1513153047</v>
       </c>
-      <c r="W263" s="1">
+      <c r="W263" s="16">
         <f t="shared" ref="W263:W284" si="9">V263/2745186691</f>
         <v>0.55120223770602561</v>
       </c>
@@ -22931,6 +23411,9 @@
       <c r="Q264" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R264" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S264" s="1">
         <v>0.95641200000000004</v>
       </c>
@@ -22940,10 +23423,10 @@
       <c r="U264" s="14">
         <v>10.205625</v>
       </c>
-      <c r="V264" s="13">
+      <c r="V264" s="17">
         <v>1697818340</v>
       </c>
-      <c r="W264" s="1">
+      <c r="W264" s="16">
         <f t="shared" si="9"/>
         <v>0.61847099345419343</v>
       </c>
@@ -23000,6 +23483,9 @@
       <c r="Q265" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R265" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S265" s="1">
         <v>0.95785200000000004</v>
       </c>
@@ -23009,10 +23495,10 @@
       <c r="U265" s="14">
         <v>10.20335</v>
       </c>
-      <c r="V265" s="13">
+      <c r="V265" s="17">
         <v>1732824237</v>
       </c>
-      <c r="W265" s="1">
+      <c r="W265" s="16">
         <f t="shared" si="9"/>
         <v>0.63122272983509808</v>
       </c>
@@ -23069,6 +23555,9 @@
       <c r="Q266" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="R266" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S266" s="1">
         <v>0.95158500000000001</v>
       </c>
@@ -23078,10 +23567,10 @@
       <c r="U266" s="14">
         <v>9.1422030000000003</v>
       </c>
-      <c r="V266" s="13">
+      <c r="V266" s="17">
         <v>1535116668</v>
       </c>
-      <c r="W266" s="1">
+      <c r="W266" s="16">
         <f t="shared" si="9"/>
         <v>0.55920301268865502</v>
       </c>
@@ -23138,6 +23627,9 @@
       <c r="Q267" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="R267" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="S267" s="13">
         <v>0.95433800000000002</v>
       </c>
@@ -23147,10 +23639,10 @@
       <c r="U267" s="15">
         <v>12.330766000000001</v>
       </c>
-      <c r="V267" s="13">
+      <c r="V267" s="17">
         <v>1862996447</v>
       </c>
-      <c r="W267" s="1">
+      <c r="W267" s="16">
         <f t="shared" si="9"/>
         <v>0.67864107497962511</v>
       </c>
@@ -23204,7 +23696,8 @@
       <c r="S268" s="13"/>
       <c r="T268" s="13"/>
       <c r="U268" s="15"/>
-      <c r="W268" s="1">
+      <c r="V268" s="18"/>
+      <c r="W268" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23285,7 +23778,8 @@
       <c r="S269" s="13"/>
       <c r="T269" s="13"/>
       <c r="U269" s="15"/>
-      <c r="W269" s="1">
+      <c r="V269" s="18"/>
+      <c r="W269" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23366,7 +23860,8 @@
       <c r="S270" s="13"/>
       <c r="T270" s="13"/>
       <c r="U270" s="15"/>
-      <c r="W270" s="1">
+      <c r="V270" s="18"/>
+      <c r="W270" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23447,7 +23942,8 @@
       <c r="S271" s="13"/>
       <c r="T271" s="13"/>
       <c r="U271" s="15"/>
-      <c r="W271" s="1">
+      <c r="V271" s="18"/>
+      <c r="W271" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23526,7 +24022,8 @@
         <v>59</v>
       </c>
       <c r="U272" s="14"/>
-      <c r="W272" s="1">
+      <c r="V272" s="18"/>
+      <c r="W272" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23605,7 +24102,8 @@
         <v>59</v>
       </c>
       <c r="U273" s="14"/>
-      <c r="W273" s="1">
+      <c r="V273" s="18"/>
+      <c r="W273" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23684,7 +24182,8 @@
         <v>59</v>
       </c>
       <c r="U274" s="14"/>
-      <c r="W274" s="1">
+      <c r="V274" s="18"/>
+      <c r="W274" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23763,7 +24262,8 @@
         <v>59</v>
       </c>
       <c r="U275" s="14"/>
-      <c r="W275" s="1">
+      <c r="V275" s="18"/>
+      <c r="W275" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23842,7 +24342,8 @@
         <v>59</v>
       </c>
       <c r="U276" s="14"/>
-      <c r="W276" s="1">
+      <c r="V276" s="18"/>
+      <c r="W276" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -23921,7 +24422,8 @@
         <v>59</v>
       </c>
       <c r="U277" s="14"/>
-      <c r="W277" s="1">
+      <c r="V277" s="18"/>
+      <c r="W277" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -24000,7 +24502,8 @@
         <v>59</v>
       </c>
       <c r="U278" s="14"/>
-      <c r="W278" s="1">
+      <c r="V278" s="18"/>
+      <c r="W278" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -24079,7 +24582,8 @@
         <v>59</v>
       </c>
       <c r="U279" s="14"/>
-      <c r="W279" s="1">
+      <c r="V279" s="18"/>
+      <c r="W279" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -24158,7 +24662,8 @@
         <v>59</v>
       </c>
       <c r="U280" s="14"/>
-      <c r="W280" s="1">
+      <c r="V280" s="18"/>
+      <c r="W280" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -24237,7 +24742,8 @@
         <v>59</v>
       </c>
       <c r="U281" s="14"/>
-      <c r="W281" s="1">
+      <c r="V281" s="18"/>
+      <c r="W281" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -24316,7 +24822,8 @@
         <v>59</v>
       </c>
       <c r="U282" s="14"/>
-      <c r="W282" s="1">
+      <c r="V282" s="18"/>
+      <c r="W282" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -24395,7 +24902,8 @@
         <v>59</v>
       </c>
       <c r="U283" s="14"/>
-      <c r="W283" s="1">
+      <c r="V283" s="18"/>
+      <c r="W283" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -24474,7 +24982,8 @@
         <v>59</v>
       </c>
       <c r="U284" s="14"/>
-      <c r="W284" s="1">
+      <c r="V284" s="18"/>
+      <c r="W284" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -24553,7 +25062,8 @@
         <v>59</v>
       </c>
       <c r="U285" s="14"/>
-      <c r="W285" s="1">
+      <c r="V285" s="18"/>
+      <c r="W285" s="16">
         <f>V285/2745186691</f>
         <v>0</v>
       </c>
@@ -24632,7 +25142,8 @@
         <v>59</v>
       </c>
       <c r="U286" s="14"/>
-      <c r="W286" s="1">
+      <c r="V286" s="18"/>
+      <c r="W286" s="16">
         <f t="shared" ref="W286:W312" si="10">V286/2745186691</f>
         <v>0</v>
       </c>
@@ -24711,7 +25222,8 @@
         <v>59</v>
       </c>
       <c r="U287" s="14"/>
-      <c r="W287" s="1">
+      <c r="V287" s="18"/>
+      <c r="W287" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -24790,7 +25302,8 @@
         <v>59</v>
       </c>
       <c r="U288" s="14"/>
-      <c r="W288" s="1">
+      <c r="V288" s="18"/>
+      <c r="W288" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -24869,7 +25382,8 @@
         <v>59</v>
       </c>
       <c r="U289" s="14"/>
-      <c r="W289" s="1">
+      <c r="V289" s="18"/>
+      <c r="W289" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -24948,7 +25462,8 @@
         <v>59</v>
       </c>
       <c r="U290" s="14"/>
-      <c r="W290" s="1">
+      <c r="V290" s="18"/>
+      <c r="W290" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25027,7 +25542,8 @@
         <v>59</v>
       </c>
       <c r="U291" s="14"/>
-      <c r="W291" s="1">
+      <c r="V291" s="18"/>
+      <c r="W291" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25106,7 +25622,8 @@
         <v>59</v>
       </c>
       <c r="U292" s="14"/>
-      <c r="W292" s="1">
+      <c r="V292" s="18"/>
+      <c r="W292" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25185,7 +25702,8 @@
         <v>59</v>
       </c>
       <c r="U293" s="14"/>
-      <c r="W293" s="1">
+      <c r="V293" s="18"/>
+      <c r="W293" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25264,7 +25782,8 @@
         <v>59</v>
       </c>
       <c r="U294" s="14"/>
-      <c r="W294" s="1">
+      <c r="V294" s="18"/>
+      <c r="W294" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25343,7 +25862,8 @@
         <v>59</v>
       </c>
       <c r="U295" s="14"/>
-      <c r="W295" s="1">
+      <c r="V295" s="18"/>
+      <c r="W295" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25422,7 +25942,8 @@
         <v>59</v>
       </c>
       <c r="U296" s="14"/>
-      <c r="W296" s="1">
+      <c r="V296" s="18"/>
+      <c r="W296" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25501,7 +26022,8 @@
         <v>59</v>
       </c>
       <c r="U297" s="14"/>
-      <c r="W297" s="1">
+      <c r="V297" s="18"/>
+      <c r="W297" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25580,7 +26102,8 @@
         <v>59</v>
       </c>
       <c r="U298" s="14"/>
-      <c r="W298" s="1">
+      <c r="V298" s="18"/>
+      <c r="W298" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25659,7 +26182,8 @@
         <v>59</v>
       </c>
       <c r="U299" s="14"/>
-      <c r="W299" s="1">
+      <c r="V299" s="18"/>
+      <c r="W299" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25738,7 +26262,8 @@
         <v>59</v>
       </c>
       <c r="U300" s="14"/>
-      <c r="W300" s="1">
+      <c r="V300" s="18"/>
+      <c r="W300" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25817,7 +26342,8 @@
         <v>59</v>
       </c>
       <c r="U301" s="14"/>
-      <c r="W301" s="1">
+      <c r="V301" s="18"/>
+      <c r="W301" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25896,7 +26422,8 @@
         <v>59</v>
       </c>
       <c r="U302" s="14"/>
-      <c r="W302" s="1">
+      <c r="V302" s="18"/>
+      <c r="W302" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -25975,7 +26502,8 @@
         <v>59</v>
       </c>
       <c r="U303" s="14"/>
-      <c r="W303" s="1">
+      <c r="V303" s="18"/>
+      <c r="W303" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26054,7 +26582,8 @@
         <v>59</v>
       </c>
       <c r="U304" s="14"/>
-      <c r="W304" s="1">
+      <c r="V304" s="18"/>
+      <c r="W304" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26133,7 +26662,8 @@
         <v>59</v>
       </c>
       <c r="U305" s="14"/>
-      <c r="W305" s="1">
+      <c r="V305" s="18"/>
+      <c r="W305" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26212,7 +26742,8 @@
         <v>59</v>
       </c>
       <c r="U306" s="14"/>
-      <c r="W306" s="1">
+      <c r="V306" s="18"/>
+      <c r="W306" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26291,7 +26822,8 @@
         <v>59</v>
       </c>
       <c r="U307" s="14"/>
-      <c r="W307" s="1">
+      <c r="V307" s="18"/>
+      <c r="W307" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26370,7 +26902,8 @@
         <v>59</v>
       </c>
       <c r="U308" s="14"/>
-      <c r="W308" s="1">
+      <c r="V308" s="18"/>
+      <c r="W308" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26449,7 +26982,8 @@
         <v>59</v>
       </c>
       <c r="U309" s="14"/>
-      <c r="W309" s="1">
+      <c r="V309" s="18"/>
+      <c r="W309" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26528,7 +27062,8 @@
         <v>59</v>
       </c>
       <c r="U310" s="14"/>
-      <c r="W310" s="1">
+      <c r="V310" s="18"/>
+      <c r="W310" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26607,7 +27142,8 @@
         <v>59</v>
       </c>
       <c r="U311" s="14"/>
-      <c r="W311" s="1">
+      <c r="V311" s="18"/>
+      <c r="W311" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26686,7 +27222,8 @@
         <v>59</v>
       </c>
       <c r="U312" s="14"/>
-      <c r="W312" s="1">
+      <c r="V312" s="18"/>
+      <c r="W312" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -26765,7 +27302,8 @@
         <v>59</v>
       </c>
       <c r="U313" s="14"/>
-      <c r="W313" s="1">
+      <c r="V313" s="18"/>
+      <c r="W313" s="16">
         <f>V313/2745186691</f>
         <v>0</v>
       </c>
@@ -26844,7 +27382,8 @@
         <v>59</v>
       </c>
       <c r="U314" s="14"/>
-      <c r="W314" s="1">
+      <c r="V314" s="18"/>
+      <c r="W314" s="16">
         <f t="shared" ref="W314:W336" si="11">V314/2745186691</f>
         <v>0</v>
       </c>
@@ -26923,7 +27462,8 @@
         <v>59</v>
       </c>
       <c r="U315" s="14"/>
-      <c r="W315" s="1">
+      <c r="V315" s="18"/>
+      <c r="W315" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27002,7 +27542,8 @@
         <v>59</v>
       </c>
       <c r="U316" s="14"/>
-      <c r="W316" s="1">
+      <c r="V316" s="18"/>
+      <c r="W316" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27081,7 +27622,8 @@
         <v>59</v>
       </c>
       <c r="U317" s="14"/>
-      <c r="W317" s="1">
+      <c r="V317" s="18"/>
+      <c r="W317" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27160,7 +27702,8 @@
         <v>59</v>
       </c>
       <c r="U318" s="14"/>
-      <c r="W318" s="1">
+      <c r="V318" s="18"/>
+      <c r="W318" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27239,7 +27782,8 @@
         <v>59</v>
       </c>
       <c r="U319" s="14"/>
-      <c r="W319" s="1">
+      <c r="V319" s="18"/>
+      <c r="W319" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27318,7 +27862,8 @@
         <v>59</v>
       </c>
       <c r="U320" s="14"/>
-      <c r="W320" s="1">
+      <c r="V320" s="18"/>
+      <c r="W320" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27397,7 +27942,8 @@
         <v>59</v>
       </c>
       <c r="U321" s="14"/>
-      <c r="W321" s="1">
+      <c r="V321" s="18"/>
+      <c r="W321" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27476,7 +28022,8 @@
         <v>59</v>
       </c>
       <c r="U322" s="14"/>
-      <c r="W322" s="1">
+      <c r="V322" s="18"/>
+      <c r="W322" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27555,7 +28102,8 @@
         <v>59</v>
       </c>
       <c r="U323" s="14"/>
-      <c r="W323" s="1">
+      <c r="V323" s="18"/>
+      <c r="W323" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27634,7 +28182,8 @@
         <v>59</v>
       </c>
       <c r="U324" s="14"/>
-      <c r="W324" s="1">
+      <c r="V324" s="18"/>
+      <c r="W324" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27713,7 +28262,8 @@
         <v>59</v>
       </c>
       <c r="U325" s="14"/>
-      <c r="W325" s="1">
+      <c r="V325" s="18"/>
+      <c r="W325" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27792,7 +28342,8 @@
         <v>59</v>
       </c>
       <c r="U326" s="14"/>
-      <c r="W326" s="1">
+      <c r="V326" s="18"/>
+      <c r="W326" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27871,7 +28422,8 @@
         <v>59</v>
       </c>
       <c r="U327" s="14"/>
-      <c r="W327" s="1">
+      <c r="V327" s="18"/>
+      <c r="W327" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27950,7 +28502,8 @@
         <v>59</v>
       </c>
       <c r="U328" s="14"/>
-      <c r="W328" s="1">
+      <c r="V328" s="18"/>
+      <c r="W328" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28029,7 +28582,8 @@
         <v>59</v>
       </c>
       <c r="U329" s="14"/>
-      <c r="W329" s="1">
+      <c r="V329" s="18"/>
+      <c r="W329" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28108,7 +28662,8 @@
         <v>59</v>
       </c>
       <c r="U330" s="14"/>
-      <c r="W330" s="1">
+      <c r="V330" s="18"/>
+      <c r="W330" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28187,7 +28742,8 @@
         <v>59</v>
       </c>
       <c r="U331" s="14"/>
-      <c r="W331" s="1">
+      <c r="V331" s="18"/>
+      <c r="W331" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28266,7 +28822,8 @@
         <v>59</v>
       </c>
       <c r="U332" s="14"/>
-      <c r="W332" s="1">
+      <c r="V332" s="18"/>
+      <c r="W332" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28345,7 +28902,8 @@
         <v>59</v>
       </c>
       <c r="U333" s="14"/>
-      <c r="W333" s="1">
+      <c r="V333" s="18"/>
+      <c r="W333" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28424,7 +28982,8 @@
         <v>59</v>
       </c>
       <c r="U334" s="14"/>
-      <c r="W334" s="1">
+      <c r="V334" s="18"/>
+      <c r="W334" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28503,7 +29062,8 @@
         <v>59</v>
       </c>
       <c r="U335" s="14"/>
-      <c r="W335" s="1">
+      <c r="V335" s="18"/>
+      <c r="W335" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28582,7 +29142,8 @@
         <v>59</v>
       </c>
       <c r="U336" s="14"/>
-      <c r="W336" s="1">
+      <c r="V336" s="18"/>
+      <c r="W336" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -28661,7 +29222,8 @@
         <v>59</v>
       </c>
       <c r="U337" s="14"/>
-      <c r="W337" s="1">
+      <c r="V337" s="18"/>
+      <c r="W337" s="16">
         <f>V337/2745186691</f>
         <v>0</v>
       </c>
@@ -28740,7 +29302,8 @@
         <v>59</v>
       </c>
       <c r="U338" s="14"/>
-      <c r="W338" s="1">
+      <c r="V338" s="18"/>
+      <c r="W338" s="16">
         <f t="shared" ref="W338:W346" si="12">V338/2745186691</f>
         <v>0</v>
       </c>
@@ -28818,7 +29381,8 @@
       <c r="O339" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W339" s="1">
+      <c r="V339" s="18"/>
+      <c r="W339" s="16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -28896,7 +29460,8 @@
       <c r="O340" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W340" s="1">
+      <c r="V340" s="18"/>
+      <c r="W340" s="16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -28974,7 +29539,8 @@
       <c r="O341" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W341" s="1">
+      <c r="V341" s="18"/>
+      <c r="W341" s="16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -29052,7 +29618,8 @@
       <c r="O342" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W342" s="1">
+      <c r="V342" s="18"/>
+      <c r="W342" s="16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -29130,7 +29697,8 @@
       <c r="O343" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W343" s="1">
+      <c r="V343" s="18"/>
+      <c r="W343" s="16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -29208,7 +29776,8 @@
       <c r="O344" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W344" s="1">
+      <c r="V344" s="18"/>
+      <c r="W344" s="16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -29286,7 +29855,8 @@
       <c r="O345" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="W345" s="1">
+      <c r="V345" s="18"/>
+      <c r="W345" s="16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -29364,7 +29934,8 @@
       <c r="O346" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="W346" s="1">
+      <c r="V346" s="18"/>
+      <c r="W346" s="16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -29395,6 +29966,51 @@
       <c r="AR346" s="1" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="347" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="V347" s="18"/>
+    </row>
+    <row r="348" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="V348" s="18"/>
+    </row>
+    <row r="349" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="V349" s="18"/>
+    </row>
+    <row r="350" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="V350" s="18"/>
+    </row>
+    <row r="351" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="V351" s="18"/>
+    </row>
+    <row r="352" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="V352" s="18"/>
+    </row>
+    <row r="353" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V353" s="18"/>
+    </row>
+    <row r="354" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V354" s="18"/>
+    </row>
+    <row r="355" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V355" s="18"/>
+    </row>
+    <row r="356" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V356" s="18"/>
+    </row>
+    <row r="357" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V357" s="18"/>
+    </row>
+    <row r="358" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V358" s="18"/>
+    </row>
+    <row r="359" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V359" s="18"/>
+    </row>
+    <row r="360" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V360" s="18"/>
+    </row>
+    <row r="361" spans="22:22" x14ac:dyDescent="0.2">
+      <c r="V361" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AM346" xr:uid="{AA242BA5-733B-FC49-A2B2-17B2B6C5E9F6}">

</xml_diff>

<commit_message>
re-did Myc translocation inspection in IGV for P3G6 and PRN4
</commit_message>
<xml_diff>
--- a/1_Input/Sample_overview.xlsx
+++ b/1_Input/Sample_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.s.steemers/surfdrive/Shared/pmc_vanboxtel/projects/Burkitt_github/1_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C399DE3-8376-734D-B372-1A854C73FA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF290A0-A939-684E-B682-397F613FAC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22660" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{42CF7DF2-1AE8-0C4E-8116-5678FAC88E91}"/>
   </bookViews>
@@ -1785,10 +1785,10 @@
   <dimension ref="A1:AR361"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W20" sqref="W20"/>
+      <selection pane="bottomRight" activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2771,7 +2771,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>420</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="S13" s="14">
         <v>0.94896100000000005</v>
@@ -3823,7 +3823,7 @@
         <v>422</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="S20" s="14">
         <v>0.55152900000000005</v>
@@ -4319,7 +4319,7 @@
         <v>419</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="S25" s="13">
         <v>0.93278300000000003</v>

</xml_diff>

<commit_message>
Reviewed Myc translocation for P3G6, PRN4 and P856
</commit_message>
<xml_diff>
--- a/1_Input/Sample_overview.xlsx
+++ b/1_Input/Sample_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.s.steemers/surfdrive/Shared/pmc_vanboxtel/projects/Burkitt_github/1_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF290A0-A939-684E-B682-397F613FAC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9628435D-0283-374A-B10E-F547DFBC766B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22660" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{42CF7DF2-1AE8-0C4E-8116-5678FAC88E91}"/>
   </bookViews>
@@ -1784,11 +1784,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA242BA5-733B-FC49-A2B2-17B2B6C5E9F6}">
   <dimension ref="A1:AR361"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="Q239" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R29" sqref="R29"/>
+      <selection pane="bottomRight" activeCell="R268" sqref="R268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21751,7 +21751,7 @@
         <v>0.58609887781945391</v>
       </c>
     </row>
-    <row r="242" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:44" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>383</v>
       </c>
@@ -22094,7 +22094,7 @@
       <c r="Q246" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="R246" s="1" t="s">
+      <c r="R246" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S246" s="14">
@@ -22167,7 +22167,7 @@
       <c r="Q247" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="R247" s="1" t="s">
+      <c r="R247" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S247" s="14">
@@ -22240,7 +22240,7 @@
       <c r="Q248" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="R248" s="1" t="s">
+      <c r="R248" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S248" s="14">
@@ -22386,7 +22386,7 @@
       <c r="Q250" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="R250" s="1" t="s">
+      <c r="R250" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S250" s="14">
@@ -22459,7 +22459,7 @@
       <c r="Q251" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="R251" s="1" t="s">
+      <c r="R251" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S251" s="14">
@@ -22532,7 +22532,7 @@
       <c r="Q252" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="R252" s="1" t="s">
+      <c r="R252" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S252" s="14">
@@ -22605,7 +22605,7 @@
       <c r="Q253" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="R253" s="1" t="s">
+      <c r="R253" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S253" s="14">
@@ -22678,7 +22678,7 @@
       <c r="Q254" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="R254" s="1" t="s">
+      <c r="R254" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S254" s="14">
@@ -22751,7 +22751,7 @@
       <c r="Q255" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R255" s="1" t="s">
+      <c r="R255" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S255" s="14">
@@ -22907,7 +22907,7 @@
       <c r="Q257" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="R257" s="1" t="s">
+      <c r="R257" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S257" s="1">
@@ -22979,7 +22979,7 @@
       <c r="Q258" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="R258" s="1" t="s">
+      <c r="R258" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S258" s="1">
@@ -23051,7 +23051,7 @@
       <c r="Q259" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="R259" s="1" t="s">
+      <c r="R259" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S259" s="1">
@@ -23411,7 +23411,7 @@
       <c r="Q264" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="R264" s="1" t="s">
+      <c r="R264" s="8" t="s">
         <v>425</v>
       </c>
       <c r="S264" s="1">

</xml_diff>

<commit_message>
Update project: add new data/code; ignore 4_Manuscript and temp files
</commit_message>
<xml_diff>
--- a/1_Input/Sample_overview.xlsx
+++ b/1_Input/Sample_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.s.steemers/surfdrive/Shared/pmc_vanboxtel/projects/Burkitt_github/1_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B726D5C7-2628-4A4A-8351-DB3A1BDB0451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E022E0-8924-4F47-A6AA-53BD3BF973D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22660" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{42CF7DF2-1AE8-0C4E-8116-5678FAC88E91}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{42CF7DF2-1AE8-0C4E-8116-5678FAC88E91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1470,6 +1492,68 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>N/A</v>
+    <v>2</v>
+    <v>6</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="argument" t="s"/>
+    <k n="errorType" t="i"/>
+    <k n="ptg" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1792,10 +1876,10 @@
   <dimension ref="A1:AS361"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="K321" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="AS6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A354" sqref="A354"/>
+      <selection pane="bottomRight" activeCell="AT1" sqref="AT1:AT1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4211,7 +4295,7 @@
       <c r="W23" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="X23" s="14" t="e">
+      <c r="X23" s="14" t="e" vm="1">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -4313,7 +4397,7 @@
       <c r="W24" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="X24" s="14" t="e">
+      <c r="X24" s="14" t="e" vm="1">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -4368,7 +4452,7 @@
         <v>114</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I25" s="2">
         <v>43837</v>
@@ -13859,7 +13943,7 @@
       <c r="W120" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="X120" s="14" t="e">
+      <c r="X120" s="14" t="e" vm="1">
         <f>W120/2745186691</f>
         <v>#VALUE!</v>
       </c>
@@ -21680,7 +21764,7 @@
       <c r="W199" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="X199" s="14" t="e">
+      <c r="X199" s="14" t="e" vm="1">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
@@ -23004,7 +23088,7 @@
       <c r="W214" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="X214" s="14" t="e">
+      <c r="X214" s="14" t="e" vm="1">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
@@ -23106,7 +23190,7 @@
       <c r="W215" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="X215" s="14" t="e">
+      <c r="X215" s="14" t="e" vm="1">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
@@ -24603,7 +24687,7 @@
       <c r="W233" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="X233" s="14" t="e">
+      <c r="X233" s="14" t="e" vm="1">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
@@ -26292,7 +26376,7 @@
       <c r="W255" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="X255" s="14" t="e">
+      <c r="X255" s="14" t="e" vm="1">
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
@@ -26379,7 +26463,7 @@
       <c r="W256" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="X256" s="14" t="e">
+      <c r="X256" s="14" t="e" vm="1">
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
@@ -34893,7 +34977,7 @@
       <c r="W345" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="X345" s="14" t="e">
+      <c r="X345" s="14" t="e" vm="1">
         <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>

</xml_diff>